<commit_message>
Working on base loading tabulation
</commit_message>
<xml_diff>
--- a/data/TEST_Values_Tables.xlsx
+++ b/data/TEST_Values_Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\Documents\R\NCZ_Interventions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD72C15-36F2-4C20-A97E-7AA59947EDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38917D0-C4CF-4BAC-8598-6E9722B84280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
   </bookViews>
@@ -340,7 +340,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -404,6 +404,44 @@
     <font>
       <b/>
       <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -492,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -591,10 +629,36 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -910,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3813FFD9-5E5D-46D2-877D-6E8E65729695}">
-  <dimension ref="C1:O126"/>
+  <dimension ref="C1:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="J121" sqref="J121"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3069,7 +3133,7 @@
       </c>
     </row>
     <row r="73" spans="3:15" x14ac:dyDescent="0.45">
-      <c r="G73" s="39">
+      <c r="G73" s="38">
         <f>SUM(G61:G72)</f>
         <v>7891121.8899999987</v>
       </c>
@@ -3969,11 +4033,11 @@
       </c>
     </row>
     <row r="104" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G104" s="40">
+      <c r="G104" s="39">
         <f>SUM(G92:G103)</f>
         <v>7891121.8899999987</v>
       </c>
-      <c r="H104" s="40">
+      <c r="H104" s="39">
         <f>SUM(H92:H103)</f>
         <v>1547396.08</v>
       </c>
@@ -3983,39 +4047,50 @@
       </c>
     </row>
     <row r="105" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D105" s="17" t="s">
+      <c r="D105" s="41" t="s">
         <v>96</v>
       </c>
+      <c r="E105" s="42"/>
+      <c r="F105" s="42"/>
+      <c r="G105" s="42"/>
+      <c r="H105" s="42"/>
+      <c r="I105" s="42"/>
+      <c r="J105" s="42"/>
+      <c r="K105" s="42"/>
+      <c r="L105" s="42"/>
+      <c r="M105" s="42"/>
+      <c r="N105" s="42"/>
     </row>
     <row r="106" spans="4:15" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E106" s="4" t="s">
+      <c r="D106" s="42"/>
+      <c r="E106" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F106" s="4" t="s">
+      <c r="F106" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="G106" s="4" t="s">
+      <c r="G106" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="H106" s="4" t="s">
+      <c r="H106" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="I106" s="4" t="s">
+      <c r="I106" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J106" s="4" t="s">
+      <c r="J106" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="K106" s="4" t="s">
+      <c r="K106" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="L106" s="4" t="s">
+      <c r="L106" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="M106" s="4" t="s">
+      <c r="M106" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="N106" s="4" t="s">
+      <c r="N106" s="44" t="s">
         <v>90</v>
       </c>
       <c r="O106" s="4" t="s">
@@ -4023,37 +4098,37 @@
       </c>
     </row>
     <row r="107" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D107" s="1">
+      <c r="D107" s="45">
         <v>217</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F107" s="3">
-        <v>1</v>
-      </c>
-      <c r="G107" s="35">
+      <c r="E107" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F107" s="47">
+        <v>1</v>
+      </c>
+      <c r="G107" s="48">
         <v>248748.087</v>
       </c>
-      <c r="H107" s="35">
+      <c r="H107" s="48">
         <v>104197.3</v>
       </c>
-      <c r="I107" s="3">
-        <v>0</v>
-      </c>
-      <c r="J107" s="3">
-        <v>0</v>
-      </c>
-      <c r="K107" s="3">
-        <v>0</v>
-      </c>
-      <c r="L107" s="3">
-        <v>0</v>
-      </c>
-      <c r="M107" s="35">
+      <c r="I107" s="47">
+        <v>0</v>
+      </c>
+      <c r="J107" s="47">
+        <v>0</v>
+      </c>
+      <c r="K107" s="47">
+        <v>0</v>
+      </c>
+      <c r="L107" s="47">
+        <v>0</v>
+      </c>
+      <c r="M107" s="48">
         <v>1004730.6</v>
       </c>
-      <c r="N107" s="3">
+      <c r="N107" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O107" s="2" t="s">
@@ -4061,37 +4136,37 @@
       </c>
     </row>
     <row r="108" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D108" s="1">
+      <c r="D108" s="45">
         <v>218</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F108" s="3">
+      <c r="E108" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F108" s="47">
         <v>2</v>
       </c>
-      <c r="G108" s="35">
+      <c r="G108" s="48">
         <v>183111.27</v>
       </c>
-      <c r="H108" s="35">
+      <c r="H108" s="48">
         <v>69624.259999999995</v>
       </c>
-      <c r="I108" s="3">
-        <v>0</v>
-      </c>
-      <c r="J108" s="3">
-        <v>0</v>
-      </c>
-      <c r="K108" s="3">
-        <v>0</v>
-      </c>
-      <c r="L108" s="3">
-        <v>0</v>
-      </c>
-      <c r="M108" s="35">
+      <c r="I108" s="47">
+        <v>0</v>
+      </c>
+      <c r="J108" s="47">
+        <v>0</v>
+      </c>
+      <c r="K108" s="47">
+        <v>0</v>
+      </c>
+      <c r="L108" s="47">
+        <v>0</v>
+      </c>
+      <c r="M108" s="48">
         <v>904520.73</v>
       </c>
-      <c r="N108" s="3">
+      <c r="N108" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O108" s="2" t="s">
@@ -4099,37 +4174,37 @@
       </c>
     </row>
     <row r="109" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D109" s="1">
+      <c r="D109" s="45">
         <v>219</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F109" s="3">
+      <c r="E109" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F109" s="47">
         <v>3</v>
       </c>
-      <c r="G109" s="35">
+      <c r="G109" s="48">
         <v>175802.98699999999</v>
       </c>
-      <c r="H109" s="35">
+      <c r="H109" s="48">
         <v>62312.41</v>
       </c>
-      <c r="I109" s="3">
-        <v>0</v>
-      </c>
-      <c r="J109" s="3">
-        <v>0</v>
-      </c>
-      <c r="K109" s="3">
-        <v>0</v>
-      </c>
-      <c r="L109" s="3">
-        <v>0</v>
-      </c>
-      <c r="M109" s="35">
+      <c r="I109" s="47">
+        <v>0</v>
+      </c>
+      <c r="J109" s="47">
+        <v>0</v>
+      </c>
+      <c r="K109" s="47">
+        <v>0</v>
+      </c>
+      <c r="L109" s="47">
+        <v>0</v>
+      </c>
+      <c r="M109" s="48">
         <v>889900.6</v>
       </c>
-      <c r="N109" s="3">
+      <c r="N109" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O109" s="2" t="s">
@@ -4137,37 +4212,37 @@
       </c>
     </row>
     <row r="110" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D110" s="1">
+      <c r="D110" s="45">
         <v>220</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F110" s="3">
+      <c r="E110" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F110" s="47">
         <v>4</v>
       </c>
-      <c r="G110" s="35">
+      <c r="G110" s="48">
         <v>95265.792000000001</v>
       </c>
-      <c r="H110" s="35">
+      <c r="H110" s="48">
         <v>26634.17</v>
       </c>
-      <c r="I110" s="3">
-        <v>0</v>
-      </c>
-      <c r="J110" s="3">
-        <v>0</v>
-      </c>
-      <c r="K110" s="3">
-        <v>0</v>
-      </c>
-      <c r="L110" s="3">
-        <v>0</v>
-      </c>
-      <c r="M110" s="35">
+      <c r="I110" s="47">
+        <v>0</v>
+      </c>
+      <c r="J110" s="47">
+        <v>0</v>
+      </c>
+      <c r="K110" s="47">
+        <v>0</v>
+      </c>
+      <c r="L110" s="47">
+        <v>0</v>
+      </c>
+      <c r="M110" s="48">
         <v>773685.17</v>
       </c>
-      <c r="N110" s="3">
+      <c r="N110" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O110" s="2" t="s">
@@ -4175,37 +4250,37 @@
       </c>
     </row>
     <row r="111" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D111" s="1">
+      <c r="D111" s="45">
         <v>221</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F111" s="3">
+      <c r="E111" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F111" s="47">
         <v>5</v>
       </c>
-      <c r="G111" s="35">
+      <c r="G111" s="48">
         <v>154994.106</v>
       </c>
-      <c r="H111" s="35">
+      <c r="H111" s="48">
         <v>21690.93</v>
       </c>
-      <c r="I111" s="3">
-        <v>0</v>
-      </c>
-      <c r="J111" s="3">
-        <v>0</v>
-      </c>
-      <c r="K111" s="3">
-        <v>0</v>
-      </c>
-      <c r="L111" s="3">
-        <v>0</v>
-      </c>
-      <c r="M111" s="35">
+      <c r="I111" s="47">
+        <v>0</v>
+      </c>
+      <c r="J111" s="47">
+        <v>0</v>
+      </c>
+      <c r="K111" s="47">
+        <v>0</v>
+      </c>
+      <c r="L111" s="47">
+        <v>0</v>
+      </c>
+      <c r="M111" s="48">
         <v>828470.23</v>
       </c>
-      <c r="N111" s="3">
+      <c r="N111" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O111" s="2" t="s">
@@ -4213,37 +4288,37 @@
       </c>
     </row>
     <row r="112" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D112" s="1">
+      <c r="D112" s="45">
         <v>222</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F112" s="3">
+      <c r="E112" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F112" s="47">
         <v>6</v>
       </c>
-      <c r="G112" s="35">
+      <c r="G112" s="48">
         <v>55308.580999999998</v>
       </c>
-      <c r="H112" s="35">
+      <c r="H112" s="48">
         <v>7322.5519999999997</v>
       </c>
-      <c r="I112" s="3">
-        <v>0</v>
-      </c>
-      <c r="J112" s="3">
-        <v>0</v>
-      </c>
-      <c r="K112" s="3">
-        <v>0</v>
-      </c>
-      <c r="L112" s="3">
-        <v>0</v>
-      </c>
-      <c r="M112" s="35">
+      <c r="I112" s="47">
+        <v>0</v>
+      </c>
+      <c r="J112" s="47">
+        <v>0</v>
+      </c>
+      <c r="K112" s="47">
+        <v>0</v>
+      </c>
+      <c r="L112" s="47">
+        <v>0</v>
+      </c>
+      <c r="M112" s="48">
         <v>714416.33</v>
       </c>
-      <c r="N112" s="3">
+      <c r="N112" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O112" s="2" t="s">
@@ -4251,37 +4326,37 @@
       </c>
     </row>
     <row r="113" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D113" s="1">
+      <c r="D113" s="45">
         <v>223</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F113" s="3">
+      <c r="E113" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F113" s="47">
         <v>7</v>
       </c>
-      <c r="G113" s="35">
+      <c r="G113" s="48">
         <v>31866.667000000001</v>
       </c>
-      <c r="H113" s="35">
+      <c r="H113" s="48">
         <v>2947.8670000000002</v>
       </c>
-      <c r="I113" s="3">
-        <v>0</v>
-      </c>
-      <c r="J113" s="3">
-        <v>0</v>
-      </c>
-      <c r="K113" s="3">
-        <v>0</v>
-      </c>
-      <c r="L113" s="3">
-        <v>0</v>
-      </c>
-      <c r="M113" s="35">
+      <c r="I113" s="47">
+        <v>0</v>
+      </c>
+      <c r="J113" s="47">
+        <v>0</v>
+      </c>
+      <c r="K113" s="47">
+        <v>0</v>
+      </c>
+      <c r="L113" s="47">
+        <v>0</v>
+      </c>
+      <c r="M113" s="48">
         <v>686599.73</v>
       </c>
-      <c r="N113" s="3">
+      <c r="N113" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O113" s="2" t="s">
@@ -4289,37 +4364,37 @@
       </c>
     </row>
     <row r="114" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D114" s="1">
+      <c r="D114" s="45">
         <v>224</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F114" s="3">
+      <c r="E114" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F114" s="47">
         <v>8</v>
       </c>
-      <c r="G114" s="35">
+      <c r="G114" s="48">
         <v>22170.692999999999</v>
       </c>
-      <c r="H114" s="35">
+      <c r="H114" s="48">
         <v>1211.674</v>
       </c>
-      <c r="I114" s="3">
-        <v>0</v>
-      </c>
-      <c r="J114" s="3">
-        <v>0</v>
-      </c>
-      <c r="K114" s="3">
-        <v>0</v>
-      </c>
-      <c r="L114" s="3">
-        <v>0</v>
-      </c>
-      <c r="M114" s="35">
+      <c r="I114" s="47">
+        <v>0</v>
+      </c>
+      <c r="J114" s="47">
+        <v>0</v>
+      </c>
+      <c r="K114" s="47">
+        <v>0</v>
+      </c>
+      <c r="L114" s="47">
+        <v>0</v>
+      </c>
+      <c r="M114" s="48">
         <v>675167.57</v>
       </c>
-      <c r="N114" s="3">
+      <c r="N114" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O114" s="2" t="s">
@@ -4327,37 +4402,37 @@
       </c>
     </row>
     <row r="115" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D115" s="1">
+      <c r="D115" s="45">
         <v>225</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F115" s="3">
+      <c r="E115" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F115" s="47">
         <v>9</v>
       </c>
-      <c r="G115" s="35">
+      <c r="G115" s="48">
         <v>184401.94200000001</v>
       </c>
-      <c r="H115" s="35">
+      <c r="H115" s="48">
         <v>17460.72</v>
       </c>
-      <c r="I115" s="3">
-        <v>0</v>
-      </c>
-      <c r="J115" s="3">
-        <v>0</v>
-      </c>
-      <c r="K115" s="3">
-        <v>0</v>
-      </c>
-      <c r="L115" s="3">
-        <v>0</v>
-      </c>
-      <c r="M115" s="35">
+      <c r="I115" s="47">
+        <v>0</v>
+      </c>
+      <c r="J115" s="47">
+        <v>0</v>
+      </c>
+      <c r="K115" s="47">
+        <v>0</v>
+      </c>
+      <c r="L115" s="47">
+        <v>0</v>
+      </c>
+      <c r="M115" s="48">
         <v>853647.87</v>
       </c>
-      <c r="N115" s="3">
+      <c r="N115" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O115" s="2" t="s">
@@ -4365,37 +4440,37 @@
       </c>
     </row>
     <row r="116" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D116" s="1">
+      <c r="D116" s="45">
         <v>226</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F116" s="3">
+      <c r="E116" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F116" s="47">
         <v>10</v>
       </c>
-      <c r="G116" s="35">
+      <c r="G116" s="48">
         <v>69508.627999999997</v>
       </c>
-      <c r="H116" s="35">
+      <c r="H116" s="48">
         <v>2603.3049999999998</v>
       </c>
-      <c r="I116" s="3">
-        <v>0</v>
-      </c>
-      <c r="J116" s="3">
-        <v>0</v>
-      </c>
-      <c r="K116" s="3">
-        <v>0</v>
-      </c>
-      <c r="L116" s="3">
-        <v>0</v>
-      </c>
-      <c r="M116" s="35">
+      <c r="I116" s="47">
+        <v>0</v>
+      </c>
+      <c r="J116" s="47">
+        <v>0</v>
+      </c>
+      <c r="K116" s="47">
+        <v>0</v>
+      </c>
+      <c r="L116" s="47">
+        <v>0</v>
+      </c>
+      <c r="M116" s="48">
         <v>723897.13</v>
       </c>
-      <c r="N116" s="3">
+      <c r="N116" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O116" s="2" t="s">
@@ -4403,37 +4478,37 @@
       </c>
     </row>
     <row r="117" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D117" s="1">
+      <c r="D117" s="45">
         <v>227</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F117" s="3">
+      <c r="E117" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F117" s="47">
         <v>11</v>
       </c>
-      <c r="G117" s="35">
+      <c r="G117" s="48">
         <v>7040483.2000000002</v>
       </c>
-      <c r="H117" s="35">
+      <c r="H117" s="48">
         <v>780939.2</v>
       </c>
-      <c r="I117" s="3">
-        <v>0</v>
-      </c>
-      <c r="J117" s="3">
-        <v>0</v>
-      </c>
-      <c r="K117" s="3">
-        <v>0</v>
-      </c>
-      <c r="L117" s="3">
-        <v>0</v>
-      </c>
-      <c r="M117" s="35">
+      <c r="I117" s="47">
+        <v>0</v>
+      </c>
+      <c r="J117" s="47">
+        <v>0</v>
+      </c>
+      <c r="K117" s="47">
+        <v>0</v>
+      </c>
+      <c r="L117" s="47">
+        <v>0</v>
+      </c>
+      <c r="M117" s="48">
         <v>651785.19999999995</v>
       </c>
-      <c r="N117" s="3">
+      <c r="N117" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O117" s="2" t="s">
@@ -4441,91 +4516,267 @@
       </c>
     </row>
     <row r="118" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
-      <c r="D118" s="1">
+      <c r="D118" s="45">
         <v>228</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F118" s="3">
+      <c r="E118" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="F118" s="47">
         <v>12</v>
       </c>
-      <c r="G118" s="35">
+      <c r="G118" s="48">
         <v>62845.065999999999</v>
       </c>
-      <c r="H118" s="35">
+      <c r="H118" s="48">
         <v>17066.5</v>
       </c>
-      <c r="I118" s="3">
-        <v>0</v>
-      </c>
-      <c r="J118" s="3">
-        <v>0</v>
-      </c>
-      <c r="K118" s="3">
-        <v>0</v>
-      </c>
-      <c r="L118" s="3">
-        <v>0</v>
-      </c>
-      <c r="M118" s="35">
+      <c r="I118" s="47">
+        <v>0</v>
+      </c>
+      <c r="J118" s="47">
+        <v>0</v>
+      </c>
+      <c r="K118" s="47">
+        <v>0</v>
+      </c>
+      <c r="L118" s="47">
+        <v>0</v>
+      </c>
+      <c r="M118" s="48">
         <v>731696.77</v>
       </c>
-      <c r="N118" s="3">
+      <c r="N118" s="49">
         <v>651785.19999999995</v>
       </c>
       <c r="O118" s="2" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="119" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D119" s="42"/>
+      <c r="E119" s="42"/>
+      <c r="F119" s="42"/>
+      <c r="G119" s="42"/>
+      <c r="H119" s="42"/>
+      <c r="I119" s="42"/>
+      <c r="J119" s="42"/>
+      <c r="K119" s="42"/>
+      <c r="L119" s="42"/>
+      <c r="M119" s="42"/>
+      <c r="N119" s="42"/>
+    </row>
     <row r="120" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G120" s="38">
+      <c r="D120" s="42"/>
+      <c r="E120" s="42"/>
+      <c r="F120" s="42"/>
+      <c r="G120" s="50">
         <f>SUM(G107:G119)</f>
         <v>8324507.0189999994</v>
       </c>
-      <c r="H120" s="38">
+      <c r="H120" s="50">
         <f>SUM(H107:H119)</f>
         <v>1114010.888</v>
       </c>
-      <c r="J120" s="31">
+      <c r="I120" s="42"/>
+      <c r="J120" s="51">
         <f>H120+G120</f>
         <v>9438517.9069999997</v>
       </c>
-      <c r="M120" s="36">
+      <c r="K120" s="42"/>
+      <c r="L120" s="42"/>
+      <c r="M120" s="52">
         <f>SUM(M107:M119)</f>
         <v>9438517.9299999997</v>
       </c>
+      <c r="N120" s="42"/>
+    </row>
+    <row r="121" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D121" s="42"/>
+      <c r="E121" s="42"/>
+      <c r="F121" s="42"/>
+      <c r="G121" s="42"/>
+      <c r="H121" s="42"/>
+      <c r="I121" s="42"/>
+      <c r="J121" s="42"/>
+      <c r="K121" s="42"/>
+      <c r="L121" s="42"/>
+      <c r="M121" s="42"/>
+      <c r="N121" s="42"/>
     </row>
     <row r="122" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G122" s="31">
+      <c r="D122" s="42"/>
+      <c r="E122" s="42"/>
+      <c r="F122" s="42"/>
+      <c r="G122" s="51">
         <f>G120-G104</f>
         <v>433385.12900000066</v>
       </c>
-      <c r="H122" s="31">
+      <c r="H122" s="51">
         <f>H104-H120</f>
         <v>433385.19200000004</v>
       </c>
+      <c r="I122" s="42"/>
+      <c r="J122" s="42"/>
+      <c r="K122" s="42"/>
+      <c r="L122" s="42"/>
+      <c r="M122" s="42"/>
+      <c r="N122" s="42"/>
     </row>
     <row r="123" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G123" s="41">
+      <c r="D123" s="42"/>
+      <c r="E123" s="42"/>
+      <c r="F123" s="42"/>
+      <c r="G123" s="53">
         <f>G122/N118</f>
         <v>0.66492017462194708</v>
       </c>
+      <c r="H123" s="42"/>
+      <c r="I123" s="42"/>
+      <c r="J123" s="42"/>
+      <c r="K123" s="42"/>
+      <c r="L123" s="42"/>
+      <c r="M123" s="42"/>
+      <c r="N123" s="42"/>
+    </row>
+    <row r="124" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D124" s="42"/>
+      <c r="E124" s="42"/>
+      <c r="F124" s="42"/>
+      <c r="G124" s="42"/>
+      <c r="H124" s="42"/>
+      <c r="I124" s="42"/>
+      <c r="J124" s="42"/>
+      <c r="K124" s="42"/>
+      <c r="L124" s="42"/>
+      <c r="M124" s="42"/>
+      <c r="N124" s="42"/>
     </row>
     <row r="125" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="H125" s="41">
+      <c r="D125" s="42"/>
+      <c r="E125" s="42"/>
+      <c r="F125" s="42"/>
+      <c r="G125" s="42"/>
+      <c r="H125" s="53">
         <f>H122/12</f>
         <v>36115.432666666668</v>
       </c>
+      <c r="I125" s="42"/>
+      <c r="J125" s="42"/>
+      <c r="K125" s="42"/>
+      <c r="L125" s="42"/>
+      <c r="M125" s="42"/>
+      <c r="N125" s="42"/>
     </row>
     <row r="126" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="H126" s="41">
+      <c r="D126" s="42"/>
+      <c r="E126" s="42"/>
+      <c r="F126" s="42"/>
+      <c r="G126" s="42"/>
+      <c r="H126" s="53">
         <f>2*H125</f>
         <v>72230.865333333335</v>
       </c>
+      <c r="I126" s="42"/>
+      <c r="J126" s="42"/>
+      <c r="K126" s="42"/>
+      <c r="L126" s="42"/>
+      <c r="M126" s="42"/>
+      <c r="N126" s="42"/>
+    </row>
+    <row r="127" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D127" s="42"/>
+      <c r="E127" s="42"/>
+      <c r="F127" s="42"/>
+      <c r="G127" s="42"/>
+      <c r="H127" s="42"/>
+      <c r="I127" s="42"/>
+      <c r="J127" s="42"/>
+      <c r="K127" s="42"/>
+      <c r="L127" s="42"/>
+      <c r="M127" s="42"/>
+      <c r="N127" s="42"/>
+    </row>
+    <row r="128" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D128" s="42"/>
+      <c r="E128" s="42"/>
+      <c r="F128" s="42"/>
+      <c r="G128" s="42"/>
+      <c r="H128" s="42"/>
+      <c r="I128" s="42"/>
+      <c r="J128" s="42"/>
+      <c r="K128" s="42"/>
+      <c r="L128" s="42"/>
+      <c r="M128" s="42"/>
+      <c r="N128" s="42"/>
+    </row>
+    <row r="129" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D129" s="42"/>
+      <c r="E129" s="42"/>
+      <c r="F129" s="42"/>
+      <c r="G129" s="42"/>
+      <c r="H129" s="42"/>
+      <c r="I129" s="42"/>
+      <c r="J129" s="42"/>
+      <c r="K129" s="42"/>
+      <c r="L129" s="42"/>
+      <c r="M129" s="42"/>
+      <c r="N129" s="42"/>
+    </row>
+    <row r="130" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D130" s="42"/>
+      <c r="E130" s="42"/>
+      <c r="F130" s="42"/>
+      <c r="G130" s="42"/>
+      <c r="H130" s="42"/>
+      <c r="I130" s="42"/>
+      <c r="J130" s="42"/>
+      <c r="K130" s="42"/>
+      <c r="L130" s="42"/>
+      <c r="M130" s="42"/>
+      <c r="N130" s="42"/>
+    </row>
+    <row r="131" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D131" s="42"/>
+      <c r="E131" s="42"/>
+      <c r="F131" s="42"/>
+      <c r="G131" s="42"/>
+      <c r="H131" s="42"/>
+      <c r="I131" s="42"/>
+      <c r="J131" s="42"/>
+      <c r="K131" s="42"/>
+      <c r="L131" s="42"/>
+      <c r="M131" s="42"/>
+      <c r="N131" s="42"/>
+    </row>
+    <row r="132" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D132" s="42"/>
+      <c r="E132" s="42"/>
+      <c r="F132" s="42"/>
+      <c r="G132" s="42"/>
+      <c r="H132" s="42"/>
+      <c r="I132" s="42"/>
+      <c r="J132" s="42"/>
+      <c r="K132" s="42"/>
+      <c r="L132" s="42"/>
+      <c r="M132" s="42"/>
+      <c r="N132" s="42"/>
+    </row>
+    <row r="133" spans="4:14" x14ac:dyDescent="0.45">
+      <c r="D133" s="40"/>
+      <c r="E133" s="40"/>
+      <c r="F133" s="40"/>
+      <c r="G133" s="40"/>
+      <c r="H133" s="40"/>
+      <c r="I133" s="40"/>
+      <c r="J133" s="40"/>
+      <c r="K133" s="40"/>
+      <c r="L133" s="40"/>
+      <c r="M133" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Getting base loads allociated right.
</commit_message>
<xml_diff>
--- a/data/TEST_Values_Tables.xlsx
+++ b/data/TEST_Values_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\Documents\R\NCZ_Interventions\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD72C15-36F2-4C20-A97E-7AA59947EDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{AAD72C15-36F2-4C20-A97E-7AA59947EDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7753DFF-9EB6-4156-9407-C42BC96AE487}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="97">
   <si>
     <t>160 Spear</t>
   </si>
@@ -340,7 +340,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +407,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -464,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -487,12 +493,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFD6DADC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD6DADC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -591,10 +608,15 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -611,6 +633,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,33 +936,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3813FFD9-5E5D-46D2-877D-6E8E65729695}">
-  <dimension ref="C1:O126"/>
+  <dimension ref="C1:O119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="J121" sqref="J121"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.46484375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" customWidth="1"/>
-    <col min="15" max="15" width="21.73046875" customWidth="1"/>
+    <col min="11" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.36328125" customWidth="1"/>
+    <col min="15" max="15" width="21.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D1" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="4:15" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="4:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
@@ -965,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D3" s="5">
         <v>1</v>
       </c>
@@ -997,7 +1023,7 @@
         <v>546785.1</v>
       </c>
     </row>
-    <row r="4" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D4" s="5">
         <v>2</v>
       </c>
@@ -1029,7 +1055,7 @@
         <v>497063.7</v>
       </c>
     </row>
-    <row r="5" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D5" s="5">
         <v>3</v>
       </c>
@@ -1061,7 +1087,7 @@
         <v>473336</v>
       </c>
     </row>
-    <row r="6" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D6" s="5">
         <v>4</v>
       </c>
@@ -1093,7 +1119,7 @@
         <v>316791</v>
       </c>
     </row>
-    <row r="7" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D7" s="5">
         <v>5</v>
       </c>
@@ -1125,7 +1151,7 @@
         <v>217587.7</v>
       </c>
     </row>
-    <row r="8" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D8" s="5">
         <v>6</v>
       </c>
@@ -1157,7 +1183,7 @@
         <v>187246.2</v>
       </c>
     </row>
-    <row r="9" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D9" s="5">
         <v>7</v>
       </c>
@@ -1189,7 +1215,7 @@
         <v>130621.4</v>
       </c>
     </row>
-    <row r="10" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D10" s="5">
         <v>8</v>
       </c>
@@ -1221,7 +1247,7 @@
         <v>70169.8</v>
       </c>
     </row>
-    <row r="11" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D11" s="5">
         <v>9</v>
       </c>
@@ -1253,7 +1279,7 @@
         <v>204523.1</v>
       </c>
     </row>
-    <row r="12" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D12" s="5">
         <v>10</v>
       </c>
@@ -1285,7 +1311,7 @@
         <v>69069.399999999994</v>
       </c>
     </row>
-    <row r="13" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D13" s="5">
         <v>11</v>
       </c>
@@ -1317,7 +1343,7 @@
         <v>101033.3</v>
       </c>
     </row>
-    <row r="14" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D14" s="5">
         <v>12</v>
       </c>
@@ -1357,7 +1383,7 @@
         <v>2956582.0999999996</v>
       </c>
     </row>
-    <row r="15" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D15" s="9">
         <v>13</v>
       </c>
@@ -1389,7 +1415,7 @@
         <v>234347.9</v>
       </c>
     </row>
-    <row r="16" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D16" s="9">
         <v>14</v>
       </c>
@@ -1421,7 +1447,7 @@
         <v>136330</v>
       </c>
     </row>
-    <row r="17" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D17" s="9">
         <v>15</v>
       </c>
@@ -1453,7 +1479,7 @@
         <v>84105.9</v>
       </c>
     </row>
-    <row r="18" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D18" s="9">
         <v>16</v>
       </c>
@@ -1485,7 +1511,7 @@
         <v>56844.1</v>
       </c>
     </row>
-    <row r="19" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D19" s="9">
         <v>17</v>
       </c>
@@ -1517,7 +1543,7 @@
         <v>41388.5</v>
       </c>
     </row>
-    <row r="20" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D20" s="9">
         <v>18</v>
       </c>
@@ -1549,7 +1575,7 @@
         <v>37157.300000000003</v>
       </c>
     </row>
-    <row r="21" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="21" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D21" s="9">
         <v>19</v>
       </c>
@@ -1581,7 +1607,7 @@
         <v>37566.800000000003</v>
       </c>
     </row>
-    <row r="22" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="22" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D22" s="9">
         <v>20</v>
       </c>
@@ -1613,7 +1639,7 @@
         <v>34420.699999999997</v>
       </c>
     </row>
-    <row r="23" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D23" s="9">
         <v>21</v>
       </c>
@@ -1645,7 +1671,7 @@
         <v>9462.5</v>
       </c>
     </row>
-    <row r="24" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D24" s="9">
         <v>22</v>
       </c>
@@ -1677,7 +1703,7 @@
         <v>1037.5</v>
       </c>
     </row>
-    <row r="25" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D25" s="9">
         <v>23</v>
       </c>
@@ -1709,7 +1735,7 @@
         <v>84060</v>
       </c>
     </row>
-    <row r="26" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="26" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D26" s="9">
         <v>24</v>
       </c>
@@ -1749,7 +1775,7 @@
         <v>851286.20000000007</v>
       </c>
     </row>
-    <row r="27" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="27" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D27" s="13">
         <v>25</v>
       </c>
@@ -1781,7 +1807,7 @@
         <v>108723.3</v>
       </c>
     </row>
-    <row r="28" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="28" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D28" s="13">
         <v>26</v>
       </c>
@@ -1813,7 +1839,7 @@
         <v>114145.7</v>
       </c>
     </row>
-    <row r="29" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="29" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D29" s="13">
         <v>27</v>
       </c>
@@ -1845,7 +1871,7 @@
         <v>141192.29999999999</v>
       </c>
     </row>
-    <row r="30" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="30" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D30" s="13">
         <v>28</v>
       </c>
@@ -1877,7 +1903,7 @@
         <v>133497.1</v>
       </c>
     </row>
-    <row r="31" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="31" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D31" s="13">
         <v>29</v>
       </c>
@@ -1909,7 +1935,7 @@
         <v>46147.9</v>
       </c>
     </row>
-    <row r="32" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D32" s="13">
         <v>30</v>
       </c>
@@ -1941,7 +1967,7 @@
         <v>26175.599999999999</v>
       </c>
     </row>
-    <row r="33" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D33" s="13">
         <v>31</v>
       </c>
@@ -1973,7 +1999,7 @@
         <v>6222.1</v>
       </c>
     </row>
-    <row r="34" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D34" s="13">
         <v>32</v>
       </c>
@@ -2005,7 +2031,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="35" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D35" s="13">
         <v>33</v>
       </c>
@@ -2037,7 +2063,7 @@
         <v>7531</v>
       </c>
     </row>
-    <row r="36" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D36" s="13">
         <v>34</v>
       </c>
@@ -2069,7 +2095,7 @@
         <v>8293.1</v>
       </c>
     </row>
-    <row r="37" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D37" s="13">
         <v>35</v>
       </c>
@@ -2101,7 +2127,7 @@
         <v>10141.5</v>
       </c>
     </row>
-    <row r="38" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D38" s="13">
         <v>36</v>
       </c>
@@ -2141,7 +2167,7 @@
         <v>834319.8</v>
       </c>
     </row>
-    <row r="40" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="4:15" x14ac:dyDescent="0.35">
       <c r="M40" t="s">
         <v>86</v>
       </c>
@@ -2154,16 +2180,16 @@
         <v>1547396.0333333332</v>
       </c>
     </row>
-    <row r="41" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="4:15" x14ac:dyDescent="0.35">
       <c r="N41" s="31"/>
       <c r="O41" s="31"/>
     </row>
-    <row r="42" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D42" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="4:15" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="4:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E43" s="4" t="s">
         <v>2</v>
       </c>
@@ -2192,7 +2218,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D44" s="1">
         <v>1</v>
       </c>
@@ -2221,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D45" s="1">
         <v>2</v>
       </c>
@@ -2250,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="46" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D46" s="1">
         <v>3</v>
       </c>
@@ -2279,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="47" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D47" s="1">
         <v>4</v>
       </c>
@@ -2308,7 +2334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="48" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D48" s="1">
         <v>5</v>
       </c>
@@ -2337,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="49" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D49" s="1">
         <v>6</v>
       </c>
@@ -2366,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="50" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D50" s="1">
         <v>7</v>
       </c>
@@ -2395,7 +2421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="51" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D51" s="1">
         <v>8</v>
       </c>
@@ -2424,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="52" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D52" s="1">
         <v>9</v>
       </c>
@@ -2453,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="53" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D53" s="1">
         <v>10</v>
       </c>
@@ -2482,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="54" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D54" s="1">
         <v>11</v>
       </c>
@@ -2511,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="55" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D55" s="1">
         <v>12</v>
       </c>
@@ -2540,7 +2566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="57" spans="4:15" x14ac:dyDescent="0.35">
       <c r="G57" s="32">
         <f>SUM(G44:G56)</f>
         <v>7891121.8899999987</v>
@@ -2550,16 +2576,16 @@
         <v>1547396.08</v>
       </c>
     </row>
-    <row r="58" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="58" spans="4:15" x14ac:dyDescent="0.35">
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
     </row>
-    <row r="59" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="59" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D59" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="4:15" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="4:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E60" s="4" t="s">
         <v>2</v>
       </c>
@@ -2588,7 +2614,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="61" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D61" s="1">
         <v>217</v>
       </c>
@@ -2628,7 +2654,7 @@
         <v>2.9999999911524355E-2</v>
       </c>
     </row>
-    <row r="62" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="62" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D62" s="1">
         <v>218</v>
       </c>
@@ -2668,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="63" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D63" s="1">
         <v>219</v>
       </c>
@@ -2708,7 +2734,7 @@
         <v>3.0000000027939677E-2</v>
       </c>
     </row>
-    <row r="64" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="64" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D64" s="1">
         <v>220</v>
       </c>
@@ -2748,7 +2774,7 @@
         <v>2.9999999911524355E-2</v>
       </c>
     </row>
-    <row r="65" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D65" s="1">
         <v>221</v>
       </c>
@@ -2788,7 +2814,7 @@
         <v>-3.0000000027939677E-2</v>
       </c>
     </row>
-    <row r="66" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D66" s="1">
         <v>222</v>
       </c>
@@ -2828,7 +2854,7 @@
         <v>1.0000000009313226E-2</v>
       </c>
     </row>
-    <row r="67" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D67" s="1">
         <v>223</v>
       </c>
@@ -2868,7 +2894,7 @@
         <v>1.0000000009313226E-2</v>
       </c>
     </row>
-    <row r="68" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="68" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D68" s="1">
         <v>224</v>
       </c>
@@ -2908,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="69" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D69" s="1">
         <v>225</v>
       </c>
@@ -2948,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="70" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D70" s="1">
         <v>226</v>
       </c>
@@ -2988,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="71" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D71" s="1">
         <v>227</v>
       </c>
@@ -3028,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="72" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D72" s="1">
         <v>228</v>
       </c>
@@ -3068,8 +3094,8 @@
         <v>-4.0000000037252903E-2</v>
       </c>
     </row>
-    <row r="73" spans="3:15" x14ac:dyDescent="0.45">
-      <c r="G73" s="39">
+    <row r="73" spans="3:15" x14ac:dyDescent="0.35">
+      <c r="G73" s="38">
         <f>SUM(G61:G72)</f>
         <v>7891121.8899999987</v>
       </c>
@@ -3078,13 +3104,13 @@
         <v>1547396.08</v>
       </c>
     </row>
-    <row r="75" spans="3:15" x14ac:dyDescent="0.45">
+    <row r="75" spans="3:15" x14ac:dyDescent="0.35">
       <c r="C75" s="37"/>
       <c r="D75" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="3:15" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E76" s="4" t="s">
         <v>2</v>
       </c>
@@ -3116,7 +3142,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="77" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D77" s="1">
         <v>219</v>
       </c>
@@ -3151,7 +3177,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="78" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="78" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D78" s="1">
         <v>220</v>
       </c>
@@ -3186,7 +3212,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="79" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="79" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D79" s="1">
         <v>221</v>
       </c>
@@ -3221,7 +3247,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="80" spans="3:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="80" spans="3:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D80" s="1">
         <v>222</v>
       </c>
@@ -3256,7 +3282,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="81" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="81" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D81" s="1">
         <v>223</v>
       </c>
@@ -3291,7 +3317,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="82" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="82" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D82" s="1">
         <v>224</v>
       </c>
@@ -3326,7 +3352,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="83" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="83" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D83" s="1">
         <v>225</v>
       </c>
@@ -3361,7 +3387,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="84" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="84" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D84" s="1">
         <v>226</v>
       </c>
@@ -3396,7 +3422,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="85" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="85" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D85" s="1">
         <v>227</v>
       </c>
@@ -3431,7 +3457,7 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="86" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="86" spans="4:15" ht="17.5" x14ac:dyDescent="0.35">
       <c r="D86" s="1">
         <v>228</v>
       </c>
@@ -3466,18 +3492,18 @@
         <v>651785.19999999995</v>
       </c>
     </row>
-    <row r="87" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="87" spans="4:15" x14ac:dyDescent="0.35">
       <c r="H87" s="31">
         <f>SUM(H77:H86)</f>
         <v>1001597.4800000001</v>
       </c>
     </row>
-    <row r="90" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="90" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D90" s="17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="91" spans="4:15" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="4:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E91" s="4" t="s">
         <v>2</v>
       </c>
@@ -3512,7 +3538,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="92" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D92">
         <v>217</v>
       </c>
@@ -3522,7 +3548,7 @@
       <c r="F92">
         <v>1</v>
       </c>
-      <c r="G92">
+      <c r="G92" s="40">
         <v>708111.83</v>
       </c>
       <c r="H92" s="25">
@@ -3550,7 +3576,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="93" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D93">
         <v>218</v>
       </c>
@@ -3560,7 +3586,7 @@
       <c r="F93">
         <v>2</v>
       </c>
-      <c r="G93">
+      <c r="G93" s="40">
         <v>655340.93000000005</v>
       </c>
       <c r="H93" s="25">
@@ -3588,7 +3614,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="94" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D94">
         <v>219</v>
       </c>
@@ -3598,7 +3624,7 @@
       <c r="F94">
         <v>3</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="40">
         <v>657022.53</v>
       </c>
       <c r="H94" s="25">
@@ -3626,7 +3652,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="95" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D95">
         <v>220</v>
       </c>
@@ -3636,7 +3662,7 @@
       <c r="F95">
         <v>4</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="40">
         <v>604641.1</v>
       </c>
       <c r="H95" s="25">
@@ -3664,7 +3690,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="96" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D96">
         <v>221</v>
       </c>
@@ -3674,7 +3700,7 @@
       <c r="F96">
         <v>5</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="40">
         <v>726762.2</v>
       </c>
       <c r="H96" s="25">
@@ -3702,7 +3728,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="97" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D97">
         <v>222</v>
       </c>
@@ -3712,7 +3738,7 @@
       <c r="F97">
         <v>6</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="40">
         <v>630889.97</v>
       </c>
       <c r="H97" s="25">
@@ -3740,7 +3766,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="98" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D98">
         <v>223</v>
       </c>
@@ -3750,7 +3776,7 @@
       <c r="F98">
         <v>7</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="40">
         <v>628462.97</v>
       </c>
       <c r="H98" s="25">
@@ -3778,7 +3804,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="99" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D99">
         <v>224</v>
       </c>
@@ -3788,7 +3814,7 @@
       <c r="F99">
         <v>8</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="40">
         <v>640180.4</v>
       </c>
       <c r="H99" s="25">
@@ -3816,7 +3842,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="100" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D100">
         <v>225</v>
       </c>
@@ -3826,7 +3852,7 @@
       <c r="F100">
         <v>9</v>
       </c>
-      <c r="G100">
+      <c r="G100" s="40">
         <v>779809</v>
       </c>
       <c r="H100" s="25">
@@ -3854,7 +3880,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="101" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="101" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D101">
         <v>226</v>
       </c>
@@ -3864,7 +3890,7 @@
       <c r="F101">
         <v>10</v>
       </c>
-      <c r="G101">
+      <c r="G101" s="40">
         <v>697763.8</v>
       </c>
       <c r="H101" s="25">
@@ -3892,7 +3918,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="102" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="102" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D102">
         <v>227</v>
       </c>
@@ -3902,7 +3928,7 @@
       <c r="F102">
         <v>11</v>
       </c>
-      <c r="G102">
+      <c r="G102" s="40">
         <v>586706.93000000005</v>
       </c>
       <c r="H102" s="25">
@@ -3930,7 +3956,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="103" spans="4:15" x14ac:dyDescent="0.35">
       <c r="D103">
         <v>228</v>
       </c>
@@ -3940,7 +3966,7 @@
       <c r="F103">
         <v>12</v>
       </c>
-      <c r="G103">
+      <c r="G103" s="40">
         <v>575430.23</v>
       </c>
       <c r="H103" s="25">
@@ -3968,560 +3994,501 @@
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G104" s="40">
+    <row r="104" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="G104" s="39">
         <f>SUM(G92:G103)</f>
         <v>7891121.8899999987</v>
       </c>
-      <c r="H104" s="40">
+      <c r="H104" s="39">
         <f>SUM(H92:H103)</f>
         <v>1547396.08</v>
       </c>
-      <c r="M104" s="25">
+      <c r="M104" s="39">
         <f>SUM(M92:M103)</f>
         <v>9438517.9299999997</v>
       </c>
-    </row>
-    <row r="105" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D105" s="17" t="s">
+      <c r="N104" s="38">
+        <f>SUM(N92:N103)</f>
+        <v>7821422.4000000013</v>
+      </c>
+    </row>
+    <row r="106" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="D106" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="4:15" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="E106" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F106" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G106" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H106" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I106" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J106" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="K106" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L106" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M106" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="N106" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="O106" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="107" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="107" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D107" s="1">
         <v>217</v>
       </c>
-      <c r="E107" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F107" s="3">
-        <v>1</v>
-      </c>
-      <c r="G107" s="35">
-        <v>248748.087</v>
-      </c>
-      <c r="H107" s="35">
-        <v>104197.3</v>
-      </c>
-      <c r="I107" s="3">
-        <v>0</v>
-      </c>
-      <c r="J107" s="3">
-        <v>0</v>
-      </c>
-      <c r="K107" s="3">
-        <v>0</v>
-      </c>
-      <c r="L107" s="3">
-        <v>0</v>
-      </c>
-      <c r="M107" s="35">
+      <c r="E107" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F107" s="42">
+        <v>1</v>
+      </c>
+      <c r="G107" s="42">
+        <v>708111.8</v>
+      </c>
+      <c r="H107" s="42">
+        <v>296618.77</v>
+      </c>
+      <c r="I107" s="42">
+        <v>0</v>
+      </c>
+      <c r="J107" s="42">
+        <v>0</v>
+      </c>
+      <c r="K107" s="42">
+        <v>0</v>
+      </c>
+      <c r="L107" s="42">
+        <v>0</v>
+      </c>
+      <c r="M107" s="42">
         <v>1004730.6</v>
       </c>
-      <c r="N107" s="3">
+      <c r="N107" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O107" s="2" t="s">
+      <c r="O107" s="41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="108" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D108" s="1">
         <v>218</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F108" s="3">
+      <c r="E108" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F108" s="42">
         <v>2</v>
       </c>
-      <c r="G108" s="35">
-        <v>183111.27</v>
-      </c>
-      <c r="H108" s="35">
-        <v>69624.259999999995</v>
-      </c>
-      <c r="I108" s="3">
-        <v>0</v>
-      </c>
-      <c r="J108" s="3">
-        <v>0</v>
-      </c>
-      <c r="K108" s="3">
-        <v>0</v>
-      </c>
-      <c r="L108" s="3">
-        <v>0</v>
-      </c>
-      <c r="M108" s="35">
-        <v>904520.73</v>
-      </c>
-      <c r="N108" s="3">
+      <c r="G108" s="42">
+        <v>655340.9</v>
+      </c>
+      <c r="H108" s="42">
+        <v>249179.8</v>
+      </c>
+      <c r="I108" s="42">
+        <v>0</v>
+      </c>
+      <c r="J108" s="42">
+        <v>0</v>
+      </c>
+      <c r="K108" s="42">
+        <v>0</v>
+      </c>
+      <c r="L108" s="42">
+        <v>0</v>
+      </c>
+      <c r="M108" s="42">
+        <v>904520.7</v>
+      </c>
+      <c r="N108" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O108" s="2" t="s">
+      <c r="O108" s="41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="109" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="109" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D109" s="1">
         <v>219</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F109" s="3">
+      <c r="E109" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F109" s="42">
         <v>3</v>
       </c>
-      <c r="G109" s="35">
-        <v>175802.98699999999</v>
-      </c>
-      <c r="H109" s="35">
-        <v>62312.41</v>
-      </c>
-      <c r="I109" s="3">
-        <v>0</v>
-      </c>
-      <c r="J109" s="3">
-        <v>0</v>
-      </c>
-      <c r="K109" s="3">
-        <v>0</v>
-      </c>
-      <c r="L109" s="3">
-        <v>0</v>
-      </c>
-      <c r="M109" s="35">
+      <c r="G109" s="42">
+        <v>657022.5</v>
+      </c>
+      <c r="H109" s="42">
+        <v>232878.07</v>
+      </c>
+      <c r="I109" s="42">
+        <v>0</v>
+      </c>
+      <c r="J109" s="42">
+        <v>0</v>
+      </c>
+      <c r="K109" s="42">
+        <v>0</v>
+      </c>
+      <c r="L109" s="42">
+        <v>0</v>
+      </c>
+      <c r="M109" s="42">
         <v>889900.6</v>
       </c>
-      <c r="N109" s="3">
+      <c r="N109" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O109" s="2" t="s">
+      <c r="O109" s="41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="110" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="110" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D110" s="1">
         <v>220</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F110" s="3">
+      <c r="E110" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F110" s="42">
         <v>4</v>
       </c>
-      <c r="G110" s="35">
-        <v>95265.792000000001</v>
-      </c>
-      <c r="H110" s="35">
-        <v>26634.17</v>
-      </c>
-      <c r="I110" s="3">
-        <v>0</v>
-      </c>
-      <c r="J110" s="3">
-        <v>0</v>
-      </c>
-      <c r="K110" s="3">
-        <v>0</v>
-      </c>
-      <c r="L110" s="3">
-        <v>0</v>
-      </c>
-      <c r="M110" s="35">
-        <v>773685.17</v>
-      </c>
-      <c r="N110" s="3">
+      <c r="G110" s="42">
+        <v>604641.1</v>
+      </c>
+      <c r="H110" s="42">
+        <v>169044.07</v>
+      </c>
+      <c r="I110" s="42">
+        <v>0</v>
+      </c>
+      <c r="J110" s="42">
+        <v>0</v>
+      </c>
+      <c r="K110" s="42">
+        <v>0</v>
+      </c>
+      <c r="L110" s="42">
+        <v>0</v>
+      </c>
+      <c r="M110" s="42">
+        <v>773685.2</v>
+      </c>
+      <c r="N110" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O110" s="2" t="s">
+      <c r="O110" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="111" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="111" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D111" s="1">
         <v>221</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F111" s="3">
+      <c r="E111" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F111" s="42">
         <v>5</v>
       </c>
-      <c r="G111" s="35">
-        <v>154994.106</v>
-      </c>
-      <c r="H111" s="35">
-        <v>21690.93</v>
-      </c>
-      <c r="I111" s="3">
-        <v>0</v>
-      </c>
-      <c r="J111" s="3">
-        <v>0</v>
-      </c>
-      <c r="K111" s="3">
-        <v>0</v>
-      </c>
-      <c r="L111" s="3">
-        <v>0</v>
-      </c>
-      <c r="M111" s="35">
-        <v>828470.23</v>
-      </c>
-      <c r="N111" s="3">
+      <c r="G111" s="42">
+        <v>726762.2</v>
+      </c>
+      <c r="H111" s="42">
+        <v>101708.03</v>
+      </c>
+      <c r="I111" s="42">
+        <v>0</v>
+      </c>
+      <c r="J111" s="42">
+        <v>0</v>
+      </c>
+      <c r="K111" s="42">
+        <v>0</v>
+      </c>
+      <c r="L111" s="42">
+        <v>0</v>
+      </c>
+      <c r="M111" s="42">
+        <v>828470.2</v>
+      </c>
+      <c r="N111" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O111" s="2" t="s">
+      <c r="O111" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="112" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="112" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D112" s="1">
         <v>222</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F112" s="3">
+      <c r="E112" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F112" s="42">
         <v>6</v>
       </c>
-      <c r="G112" s="35">
-        <v>55308.580999999998</v>
-      </c>
-      <c r="H112" s="35">
-        <v>7322.5519999999997</v>
-      </c>
-      <c r="I112" s="3">
-        <v>0</v>
-      </c>
-      <c r="J112" s="3">
-        <v>0</v>
-      </c>
-      <c r="K112" s="3">
-        <v>0</v>
-      </c>
-      <c r="L112" s="3">
-        <v>0</v>
-      </c>
-      <c r="M112" s="35">
-        <v>714416.33</v>
-      </c>
-      <c r="N112" s="3">
+      <c r="G112" s="42">
+        <v>630890</v>
+      </c>
+      <c r="H112" s="42">
+        <v>83526.37</v>
+      </c>
+      <c r="I112" s="42">
+        <v>0</v>
+      </c>
+      <c r="J112" s="42">
+        <v>0</v>
+      </c>
+      <c r="K112" s="42">
+        <v>0</v>
+      </c>
+      <c r="L112" s="42">
+        <v>0</v>
+      </c>
+      <c r="M112" s="42">
+        <v>714416.3</v>
+      </c>
+      <c r="N112" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O112" s="2" t="s">
+      <c r="O112" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="113" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="113" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D113" s="1">
         <v>223</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F113" s="3">
+      <c r="E113" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F113" s="42">
         <v>7</v>
       </c>
-      <c r="G113" s="35">
-        <v>31866.667000000001</v>
-      </c>
-      <c r="H113" s="35">
-        <v>2947.8670000000002</v>
-      </c>
-      <c r="I113" s="3">
-        <v>0</v>
-      </c>
-      <c r="J113" s="3">
-        <v>0</v>
-      </c>
-      <c r="K113" s="3">
-        <v>0</v>
-      </c>
-      <c r="L113" s="3">
-        <v>0</v>
-      </c>
-      <c r="M113" s="35">
-        <v>686599.73</v>
-      </c>
-      <c r="N113" s="3">
+      <c r="G113" s="42">
+        <v>628463</v>
+      </c>
+      <c r="H113" s="42">
+        <v>58136.77</v>
+      </c>
+      <c r="I113" s="42">
+        <v>0</v>
+      </c>
+      <c r="J113" s="42">
+        <v>0</v>
+      </c>
+      <c r="K113" s="42">
+        <v>0</v>
+      </c>
+      <c r="L113" s="42">
+        <v>0</v>
+      </c>
+      <c r="M113" s="42">
+        <v>686599.7</v>
+      </c>
+      <c r="N113" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O113" s="2" t="s">
+      <c r="O113" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="114" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="114" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D114" s="1">
         <v>224</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F114" s="3">
+      <c r="E114" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F114" s="42">
         <v>8</v>
       </c>
-      <c r="G114" s="35">
-        <v>22170.692999999999</v>
-      </c>
-      <c r="H114" s="35">
-        <v>1211.674</v>
-      </c>
-      <c r="I114" s="3">
-        <v>0</v>
-      </c>
-      <c r="J114" s="3">
-        <v>0</v>
-      </c>
-      <c r="K114" s="3">
-        <v>0</v>
-      </c>
-      <c r="L114" s="3">
-        <v>0</v>
-      </c>
-      <c r="M114" s="35">
-        <v>675167.57</v>
-      </c>
-      <c r="N114" s="3">
+      <c r="G114" s="42">
+        <v>640180.4</v>
+      </c>
+      <c r="H114" s="42">
+        <v>34987.17</v>
+      </c>
+      <c r="I114" s="42">
+        <v>0</v>
+      </c>
+      <c r="J114" s="42">
+        <v>0</v>
+      </c>
+      <c r="K114" s="42">
+        <v>0</v>
+      </c>
+      <c r="L114" s="42">
+        <v>0</v>
+      </c>
+      <c r="M114" s="42">
+        <v>675167.6</v>
+      </c>
+      <c r="N114" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O114" s="2" t="s">
+      <c r="O114" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="115" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="115" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D115" s="1">
         <v>225</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F115" s="3">
+      <c r="E115" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F115" s="42">
         <v>9</v>
       </c>
-      <c r="G115" s="35">
-        <v>184401.94200000001</v>
-      </c>
-      <c r="H115" s="35">
-        <v>17460.72</v>
-      </c>
-      <c r="I115" s="3">
-        <v>0</v>
-      </c>
-      <c r="J115" s="3">
-        <v>0</v>
-      </c>
-      <c r="K115" s="3">
-        <v>0</v>
-      </c>
-      <c r="L115" s="3">
-        <v>0</v>
-      </c>
-      <c r="M115" s="35">
-        <v>853647.87</v>
-      </c>
-      <c r="N115" s="3">
+      <c r="G115" s="42">
+        <v>779809</v>
+      </c>
+      <c r="H115" s="42">
+        <v>73838.87</v>
+      </c>
+      <c r="I115" s="42">
+        <v>0</v>
+      </c>
+      <c r="J115" s="42">
+        <v>0</v>
+      </c>
+      <c r="K115" s="42">
+        <v>0</v>
+      </c>
+      <c r="L115" s="42">
+        <v>0</v>
+      </c>
+      <c r="M115" s="42">
+        <v>853647.9</v>
+      </c>
+      <c r="N115" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O115" s="2" t="s">
+      <c r="O115" s="41" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="116" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="116" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D116" s="1">
         <v>226</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F116" s="3">
+      <c r="E116" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F116" s="42">
         <v>10</v>
       </c>
-      <c r="G116" s="35">
-        <v>69508.627999999997</v>
-      </c>
-      <c r="H116" s="35">
-        <v>2603.3049999999998</v>
-      </c>
-      <c r="I116" s="3">
-        <v>0</v>
-      </c>
-      <c r="J116" s="3">
-        <v>0</v>
-      </c>
-      <c r="K116" s="3">
-        <v>0</v>
-      </c>
-      <c r="L116" s="3">
-        <v>0</v>
-      </c>
-      <c r="M116" s="35">
-        <v>723897.13</v>
-      </c>
-      <c r="N116" s="3">
+      <c r="G116" s="42">
+        <v>697763.8</v>
+      </c>
+      <c r="H116" s="42">
+        <v>26133.33</v>
+      </c>
+      <c r="I116" s="42">
+        <v>0</v>
+      </c>
+      <c r="J116" s="42">
+        <v>0</v>
+      </c>
+      <c r="K116" s="42">
+        <v>0</v>
+      </c>
+      <c r="L116" s="42">
+        <v>0</v>
+      </c>
+      <c r="M116" s="42">
+        <v>723897.1</v>
+      </c>
+      <c r="N116" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O116" s="2" t="s">
+      <c r="O116" s="41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="117" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="117" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D117" s="1">
         <v>227</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F117" s="3">
+      <c r="E117" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F117" s="42">
         <v>11</v>
       </c>
-      <c r="G117" s="35">
-        <v>7040483.2000000002</v>
-      </c>
-      <c r="H117" s="35">
-        <v>780939.2</v>
-      </c>
-      <c r="I117" s="3">
-        <v>0</v>
-      </c>
-      <c r="J117" s="3">
-        <v>0</v>
-      </c>
-      <c r="K117" s="3">
-        <v>0</v>
-      </c>
-      <c r="L117" s="3">
-        <v>0</v>
-      </c>
-      <c r="M117" s="35">
+      <c r="G117" s="42">
+        <v>586706.9</v>
+      </c>
+      <c r="H117" s="42">
+        <v>65078.27</v>
+      </c>
+      <c r="I117" s="42">
+        <v>0</v>
+      </c>
+      <c r="J117" s="42">
+        <v>0</v>
+      </c>
+      <c r="K117" s="42">
+        <v>0</v>
+      </c>
+      <c r="L117" s="42">
+        <v>0</v>
+      </c>
+      <c r="M117" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="N117" s="3">
+      <c r="N117" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O117" s="2" t="s">
+      <c r="O117" s="41" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="118" spans="4:15" ht="18.75" x14ac:dyDescent="0.45">
+    <row r="118" spans="4:15" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D118" s="1">
         <v>228</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F118" s="3">
+      <c r="E118" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F118" s="42">
         <v>12</v>
       </c>
-      <c r="G118" s="35">
-        <v>62845.065999999999</v>
-      </c>
-      <c r="H118" s="35">
-        <v>17066.5</v>
-      </c>
-      <c r="I118" s="3">
-        <v>0</v>
-      </c>
-      <c r="J118" s="3">
-        <v>0</v>
-      </c>
-      <c r="K118" s="3">
-        <v>0</v>
-      </c>
-      <c r="L118" s="3">
-        <v>0</v>
-      </c>
-      <c r="M118" s="35">
-        <v>731696.77</v>
-      </c>
-      <c r="N118" s="3">
+      <c r="G118" s="42">
+        <v>575430.19999999995</v>
+      </c>
+      <c r="H118" s="42">
+        <v>156266.53</v>
+      </c>
+      <c r="I118" s="42">
+        <v>0</v>
+      </c>
+      <c r="J118" s="42">
+        <v>0</v>
+      </c>
+      <c r="K118" s="42">
+        <v>0</v>
+      </c>
+      <c r="L118" s="42">
+        <v>0</v>
+      </c>
+      <c r="M118" s="42">
+        <v>731696.8</v>
+      </c>
+      <c r="N118" s="42">
         <v>651785.19999999995</v>
       </c>
-      <c r="O118" s="2" t="s">
+      <c r="O118" s="41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G120" s="38">
-        <f>SUM(G107:G119)</f>
-        <v>8324507.0189999994</v>
-      </c>
-      <c r="H120" s="38">
-        <f>SUM(H107:H119)</f>
-        <v>1114010.888</v>
-      </c>
-      <c r="J120" s="31">
-        <f>H120+G120</f>
-        <v>9438517.9069999997</v>
-      </c>
-      <c r="M120" s="36">
-        <f>SUM(M107:M119)</f>
-        <v>9438517.9299999997</v>
-      </c>
-    </row>
-    <row r="122" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G122" s="31">
-        <f>G120-G104</f>
-        <v>433385.12900000066</v>
-      </c>
-      <c r="H122" s="31">
-        <f>H104-H120</f>
-        <v>433385.19200000004</v>
-      </c>
-    </row>
-    <row r="123" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="G123" s="41">
-        <f>G122/N118</f>
-        <v>0.66492017462194708</v>
-      </c>
-    </row>
-    <row r="125" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="H125" s="41">
-        <f>H122/12</f>
-        <v>36115.432666666668</v>
-      </c>
-    </row>
-    <row r="126" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="H126" s="41">
-        <f>2*H125</f>
-        <v>72230.865333333335</v>
+    <row r="119" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="G119" s="38">
+        <f>SUM(G107:G118)</f>
+        <v>7891121.8000000007</v>
+      </c>
+      <c r="H119" s="38">
+        <f>SUM(H107:H118)</f>
+        <v>1547396.0500000005</v>
+      </c>
+      <c r="M119" s="38">
+        <f>SUM(M107:M118)</f>
+        <v>9438517.9000000004</v>
+      </c>
+      <c r="N119" s="38">
+        <f>SUM(N107:N118)</f>
+        <v>7821422.4000000013</v>
       </c>
     </row>
   </sheetData>
@@ -4537,30 +4504,30 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="12.06640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.59765625" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.08984375" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C4" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C5" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C6" s="19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="3:5" ht="23.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:5" ht="24" x14ac:dyDescent="0.35">
       <c r="C9" s="20" t="s">
         <v>15</v>
       </c>
@@ -4571,7 +4538,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C10" s="21" t="s">
         <v>18</v>
       </c>
@@ -4582,7 +4549,7 @@
         <v>329554.90000000002</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C11" s="21" t="s">
         <v>19</v>
       </c>
@@ -4593,7 +4560,7 @@
         <v>328978.2</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C12" s="21" t="s">
         <v>20</v>
       </c>
@@ -4604,7 +4571,7 @@
         <v>69270.8</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C13" s="21" t="s">
         <v>21</v>
       </c>
@@ -4615,7 +4582,7 @@
         <v>214232.2</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C14" s="21" t="s">
         <v>22</v>
       </c>
@@ -4626,7 +4593,7 @@
         <v>234298.8</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C15" s="21" t="s">
         <v>23</v>
       </c>
@@ -4637,7 +4604,7 @@
         <v>215427</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C16" s="21" t="s">
         <v>24</v>
       </c>
@@ -4648,7 +4615,7 @@
         <v>286371</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C17" s="21" t="s">
         <v>25</v>
       </c>
@@ -4659,7 +4626,7 @@
         <v>311303.5</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" s="22" t="s">
         <v>26</v>
       </c>
@@ -4670,7 +4637,7 @@
         <v>546785.1</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="22" t="s">
         <v>27</v>
       </c>
@@ -4681,7 +4648,7 @@
         <v>497063.7</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="22" t="s">
         <v>28</v>
       </c>
@@ -4692,7 +4659,7 @@
         <v>473336</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="22" t="s">
         <v>29</v>
       </c>
@@ -4703,7 +4670,7 @@
         <v>316791</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="22" t="s">
         <v>30</v>
       </c>
@@ -4714,7 +4681,7 @@
         <v>217587.7</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="22" t="s">
         <v>31</v>
       </c>
@@ -4725,7 +4692,7 @@
         <v>187246.2</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="22" t="s">
         <v>32</v>
       </c>
@@ -4736,7 +4703,7 @@
         <v>130621.4</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="22" t="s">
         <v>33</v>
       </c>
@@ -4747,7 +4714,7 @@
         <v>70169.8</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="22" t="s">
         <v>34</v>
       </c>
@@ -4758,7 +4725,7 @@
         <v>204523.1</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="22" t="s">
         <v>35</v>
       </c>
@@ -4769,7 +4736,7 @@
         <v>69069.399999999994</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="22" t="s">
         <v>36</v>
       </c>
@@ -4780,7 +4747,7 @@
         <v>101033.3</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="22" t="s">
         <v>37</v>
       </c>
@@ -4799,7 +4766,7 @@
         <v>2956582.0999999996</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="23" t="s">
         <v>38</v>
       </c>
@@ -4812,7 +4779,7 @@
       <c r="F30" s="25"/>
       <c r="G30" s="25"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="23" t="s">
         <v>39</v>
       </c>
@@ -4825,7 +4792,7 @@
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="23" t="s">
         <v>40</v>
       </c>
@@ -4838,7 +4805,7 @@
       <c r="F32" s="25"/>
       <c r="G32" s="25"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="23" t="s">
         <v>41</v>
       </c>
@@ -4851,7 +4818,7 @@
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="23" t="s">
         <v>42</v>
       </c>
@@ -4864,7 +4831,7 @@
       <c r="F34" s="25"/>
       <c r="G34" s="25"/>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="23" t="s">
         <v>43</v>
       </c>
@@ -4877,7 +4844,7 @@
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="23" t="s">
         <v>44</v>
       </c>
@@ -4890,7 +4857,7 @@
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="23" t="s">
         <v>45</v>
       </c>
@@ -4903,7 +4870,7 @@
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="23" t="s">
         <v>46</v>
       </c>
@@ -4916,7 +4883,7 @@
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="23" t="s">
         <v>47</v>
       </c>
@@ -4929,7 +4896,7 @@
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="23" t="s">
         <v>48</v>
       </c>
@@ -4942,7 +4909,7 @@
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="23" t="s">
         <v>49</v>
       </c>
@@ -4961,7 +4928,7 @@
         <v>851286.20000000007</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="24" t="s">
         <v>50</v>
       </c>
@@ -4974,7 +4941,7 @@
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="24" t="s">
         <v>51</v>
       </c>
@@ -4987,7 +4954,7 @@
       <c r="F43" s="25"/>
       <c r="G43" s="25"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="24" t="s">
         <v>52</v>
       </c>
@@ -5000,7 +4967,7 @@
       <c r="F44" s="25"/>
       <c r="G44" s="25"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="24" t="s">
         <v>53</v>
       </c>
@@ -5013,7 +4980,7 @@
       <c r="F45" s="25"/>
       <c r="G45" s="25"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="24" t="s">
         <v>54</v>
       </c>
@@ -5026,7 +4993,7 @@
       <c r="F46" s="25"/>
       <c r="G46" s="25"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="24" t="s">
         <v>55</v>
       </c>
@@ -5039,7 +5006,7 @@
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="24" t="s">
         <v>56</v>
       </c>
@@ -5052,7 +5019,7 @@
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="24" t="s">
         <v>57</v>
       </c>
@@ -5065,7 +5032,7 @@
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="24" t="s">
         <v>58</v>
       </c>
@@ -5078,7 +5045,7 @@
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="24" t="s">
         <v>59</v>
       </c>
@@ -5091,7 +5058,7 @@
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="24" t="s">
         <v>60</v>
       </c>
@@ -5104,7 +5071,7 @@
       <c r="F52" s="25"/>
       <c r="G52" s="25"/>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="24" t="s">
         <v>61</v>
       </c>
@@ -5123,7 +5090,7 @@
         <v>834319.8</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="21" t="s">
         <v>62</v>
       </c>
@@ -5136,7 +5103,7 @@
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="21" t="s">
         <v>63</v>
       </c>
@@ -5147,7 +5114,7 @@
         <v>298089.5</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="21" t="s">
         <v>64</v>
       </c>
@@ -5158,7 +5125,7 @@
         <v>191712.7</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="21" t="s">
         <v>65</v>
       </c>
@@ -5169,7 +5136,7 @@
         <v>176191</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="21" t="s">
         <v>66</v>
       </c>
@@ -5180,7 +5147,7 @@
         <v>122674.4</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="21" t="s">
         <v>67</v>
       </c>
@@ -5191,7 +5158,7 @@
         <v>70599</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="21" t="s">
         <v>68</v>
       </c>
@@ -5202,7 +5169,7 @@
         <v>66973.3</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="21" t="s">
         <v>69</v>
       </c>
@@ -5213,7 +5180,7 @@
         <v>57715.199999999997</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="21" t="s">
         <v>70</v>
       </c>
@@ -5224,7 +5191,7 @@
         <v>45198.8</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="21" t="s">
         <v>71</v>
       </c>
@@ -5235,7 +5202,7 @@
         <v>118806.9</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="21" t="s">
         <v>72</v>
       </c>
@@ -5246,7 +5213,7 @@
         <v>235342.1</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C65" s="21" t="s">
         <v>73</v>
       </c>
@@ -5257,7 +5224,7 @@
         <v>357820</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C66" s="21" t="s">
         <v>74</v>
       </c>
@@ -5268,7 +5235,7 @@
         <v>379797.1</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C67" s="21" t="s">
         <v>75</v>
       </c>
@@ -5279,7 +5246,7 @@
         <v>347400.8</v>
       </c>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C68" s="21" t="s">
         <v>76</v>
       </c>
@@ -5290,7 +5257,7 @@
         <v>379081.5</v>
       </c>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C69" s="21" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
getting git up to date
</commit_message>
<xml_diff>
--- a/data/TEST_Values_Tables.xlsx
+++ b/data/TEST_Values_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{35015F2C-5694-4A86-B3A9-A4D61B86BB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF246737-68B0-4301-B415-D2FF725AAFD6}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{35015F2C-5694-4A86-B3A9-A4D61B86BB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7495ED9-2FCC-412F-A56A-4878526BB53F}"/>
   <bookViews>
-    <workbookView xWindow="2470" yWindow="3810" windowWidth="16920" windowHeight="10540" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
+    <workbookView xWindow="7380" yWindow="3540" windowWidth="16920" windowHeight="10540" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="124">
   <si>
     <t>160 Spear</t>
   </si>
@@ -385,6 +385,33 @@
   </si>
   <si>
     <t>Electric Base Loads</t>
+  </si>
+  <si>
+    <t>UP TO LINE 72</t>
+  </si>
+  <si>
+    <t>UP TO 123</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>NGas</t>
+  </si>
+  <si>
+    <t>UP TO 142</t>
+  </si>
+  <si>
+    <t>UP TO 162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UP TO  180 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to get interventions into different sheets in the main inervention  excel file. </t>
   </si>
 </sst>
 </file>
@@ -395,7 +422,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +499,46 @@
       <b/>
       <sz val="6"/>
       <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFB0B0B0"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -676,7 +743,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -800,17 +867,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -843,7 +933,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>493889</xdr:colOff>
       <xdr:row>133</xdr:row>
-      <xdr:rowOff>68585</xdr:rowOff>
+      <xdr:rowOff>68547</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -877,6 +967,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1176,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3813FFD9-5E5D-46D2-877D-6E8E65729695}">
-  <dimension ref="C1:Y181"/>
+  <dimension ref="C1:Z201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D173" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H183" sqref="H183"/>
+    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="126" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5006,1067 +5100,1679 @@
         <v>3.4179997310840089</v>
       </c>
     </row>
-    <row r="159" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D159" s="43">
-        <v>1</v>
-      </c>
-      <c r="E159" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F159" s="42">
-        <v>1</v>
-      </c>
-      <c r="G159" s="42">
+    <row r="158" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D158" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="160" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D160" s="57">
+        <v>1</v>
+      </c>
+      <c r="E160" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F160" s="59">
+        <v>1</v>
+      </c>
+      <c r="G160" s="59">
         <v>708111.8</v>
       </c>
-      <c r="H159" s="42">
+      <c r="H160" s="59">
         <v>296618.77</v>
       </c>
-      <c r="I159" s="42">
-        <v>0</v>
-      </c>
-      <c r="J159" s="42">
-        <v>0</v>
-      </c>
-      <c r="K159" s="42">
-        <v>0</v>
-      </c>
-      <c r="L159" s="42">
-        <v>0</v>
-      </c>
-      <c r="M159" s="42">
+      <c r="I160" s="59">
+        <v>0</v>
+      </c>
+      <c r="J160" s="59">
+        <v>0</v>
+      </c>
+      <c r="K160" s="59">
+        <v>0</v>
+      </c>
+      <c r="L160" s="59">
+        <v>0</v>
+      </c>
+      <c r="M160" s="59">
         <v>1004730.6</v>
       </c>
-      <c r="N159" s="42">
+      <c r="N160" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O159" s="42">
+      <c r="O160" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P159" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q159" s="42">
-        <v>0</v>
-      </c>
-      <c r="R159" s="42">
-        <v>0</v>
-      </c>
-      <c r="S159" s="42">
-        <v>0</v>
-      </c>
-      <c r="T159" s="41" t="s">
+      <c r="P160" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q160" s="59">
+        <v>0</v>
+      </c>
+      <c r="R160" s="59">
+        <v>0</v>
+      </c>
+      <c r="S160" s="59">
+        <v>0</v>
+      </c>
+      <c r="T160" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U159" s="41" t="s">
+      <c r="U160" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V159" s="41" t="s">
+      <c r="V160" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W159" s="41" t="s">
+      <c r="W160" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X159" s="41" t="s">
+      <c r="X160" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y159" s="41" t="s">
+      <c r="Y160" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="160" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D160" s="43">
+    <row r="161" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D161" s="57">
         <v>2</v>
       </c>
-      <c r="E160" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F160" s="42">
+      <c r="E161" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F161" s="59">
         <v>2</v>
       </c>
-      <c r="G160" s="42">
+      <c r="G161" s="59">
         <v>655340.9</v>
       </c>
-      <c r="H160" s="42">
+      <c r="H161" s="59">
         <v>249179.8</v>
       </c>
-      <c r="I160" s="42">
-        <v>0</v>
-      </c>
-      <c r="J160" s="42">
-        <v>0</v>
-      </c>
-      <c r="K160" s="42">
-        <v>0</v>
-      </c>
-      <c r="L160" s="42">
-        <v>0</v>
-      </c>
-      <c r="M160" s="42">
+      <c r="I161" s="59">
+        <v>0</v>
+      </c>
+      <c r="J161" s="59">
+        <v>0</v>
+      </c>
+      <c r="K161" s="59">
+        <v>0</v>
+      </c>
+      <c r="L161" s="59">
+        <v>0</v>
+      </c>
+      <c r="M161" s="59">
         <v>904520.7</v>
       </c>
-      <c r="N160" s="42">
+      <c r="N161" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O160" s="42">
+      <c r="O161" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P160" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q160" s="42">
-        <v>0</v>
-      </c>
-      <c r="R160" s="42">
-        <v>0</v>
-      </c>
-      <c r="S160" s="42">
-        <v>0</v>
-      </c>
-      <c r="T160" s="41" t="s">
+      <c r="P161" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q161" s="59">
+        <v>0</v>
+      </c>
+      <c r="R161" s="59">
+        <v>0</v>
+      </c>
+      <c r="S161" s="59">
+        <v>0</v>
+      </c>
+      <c r="T161" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U160" s="41" t="s">
+      <c r="U161" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V160" s="41" t="s">
+      <c r="V161" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W160" s="41" t="s">
+      <c r="W161" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X160" s="41" t="s">
+      <c r="X161" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y160" s="41" t="s">
+      <c r="Y161" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="161" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D161" s="43">
+    <row r="162" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D162" s="57">
         <v>3</v>
       </c>
-      <c r="E161" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F161" s="42">
+      <c r="E162" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F162" s="59">
         <v>3</v>
       </c>
-      <c r="G161" s="42">
+      <c r="G162" s="59">
         <v>657022.5</v>
       </c>
-      <c r="H161" s="42">
+      <c r="H162" s="59">
         <v>232878.07</v>
       </c>
-      <c r="I161" s="42">
-        <v>0</v>
-      </c>
-      <c r="J161" s="42">
-        <v>0</v>
-      </c>
-      <c r="K161" s="42">
-        <v>0</v>
-      </c>
-      <c r="L161" s="42">
-        <v>0</v>
-      </c>
-      <c r="M161" s="42">
+      <c r="I162" s="59">
+        <v>0</v>
+      </c>
+      <c r="J162" s="59">
+        <v>0</v>
+      </c>
+      <c r="K162" s="59">
+        <v>0</v>
+      </c>
+      <c r="L162" s="59">
+        <v>0</v>
+      </c>
+      <c r="M162" s="59">
         <v>889900.6</v>
       </c>
-      <c r="N161" s="42">
+      <c r="N162" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O161" s="42">
+      <c r="O162" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P161" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q161" s="42">
-        <v>0</v>
-      </c>
-      <c r="R161" s="42">
-        <v>0</v>
-      </c>
-      <c r="S161" s="42">
-        <v>0</v>
-      </c>
-      <c r="T161" s="41" t="s">
+      <c r="P162" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q162" s="59">
+        <v>0</v>
+      </c>
+      <c r="R162" s="59">
+        <v>0</v>
+      </c>
+      <c r="S162" s="59">
+        <v>0</v>
+      </c>
+      <c r="T162" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U161" s="41" t="s">
+      <c r="U162" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V161" s="41" t="s">
+      <c r="V162" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W161" s="41" t="s">
+      <c r="W162" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X161" s="41" t="s">
+      <c r="X162" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y161" s="41" t="s">
+      <c r="Y162" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="162" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D162" s="43">
+    <row r="163" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D163" s="57">
         <v>4</v>
       </c>
-      <c r="E162" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F162" s="42">
+      <c r="E163" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F163" s="59">
         <v>4</v>
       </c>
-      <c r="G162" s="42">
+      <c r="G163" s="59">
         <v>604641.1</v>
       </c>
-      <c r="H162" s="42">
+      <c r="H163" s="59">
         <v>169044.07</v>
       </c>
-      <c r="I162" s="42">
-        <v>0</v>
-      </c>
-      <c r="J162" s="42">
-        <v>0</v>
-      </c>
-      <c r="K162" s="42">
-        <v>0</v>
-      </c>
-      <c r="L162" s="42">
-        <v>0</v>
-      </c>
-      <c r="M162" s="42">
+      <c r="I163" s="59">
+        <v>0</v>
+      </c>
+      <c r="J163" s="59">
+        <v>0</v>
+      </c>
+      <c r="K163" s="59">
+        <v>0</v>
+      </c>
+      <c r="L163" s="59">
+        <v>0</v>
+      </c>
+      <c r="M163" s="59">
         <v>773685.2</v>
       </c>
-      <c r="N162" s="42">
+      <c r="N163" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O162" s="42">
+      <c r="O163" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P162" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q162" s="42">
-        <v>0</v>
-      </c>
-      <c r="R162" s="42">
-        <v>0</v>
-      </c>
-      <c r="S162" s="42">
-        <v>0</v>
-      </c>
-      <c r="T162" s="41" t="s">
+      <c r="P163" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="59">
+        <v>0</v>
+      </c>
+      <c r="R163" s="59">
+        <v>0</v>
+      </c>
+      <c r="S163" s="59">
+        <v>0</v>
+      </c>
+      <c r="T163" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="U162" s="41" t="s">
+      <c r="U163" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="V162" s="41" t="s">
+      <c r="V163" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W162" s="41" t="s">
+      <c r="W163" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X162" s="41" t="s">
+      <c r="X163" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y162" s="41" t="s">
+      <c r="Y163" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="163" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D163" s="43">
+    <row r="164" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D164" s="57">
         <v>5</v>
       </c>
-      <c r="E163" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F163" s="42">
+      <c r="E164" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F164" s="59">
         <v>5</v>
       </c>
-      <c r="G163" s="42">
+      <c r="G164" s="59">
         <v>726762.2</v>
       </c>
-      <c r="H163" s="42">
+      <c r="H164" s="59">
         <v>101708.03</v>
       </c>
-      <c r="I163" s="42">
-        <v>0</v>
-      </c>
-      <c r="J163" s="42">
-        <v>0</v>
-      </c>
-      <c r="K163" s="42">
-        <v>0</v>
-      </c>
-      <c r="L163" s="42">
-        <v>0</v>
-      </c>
-      <c r="M163" s="42">
+      <c r="I164" s="59">
+        <v>0</v>
+      </c>
+      <c r="J164" s="59">
+        <v>0</v>
+      </c>
+      <c r="K164" s="59">
+        <v>0</v>
+      </c>
+      <c r="L164" s="59">
+        <v>0</v>
+      </c>
+      <c r="M164" s="59">
         <v>828470.2</v>
       </c>
-      <c r="N163" s="42">
+      <c r="N164" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O163" s="42">
+      <c r="O164" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P163" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q163" s="42">
-        <v>0</v>
-      </c>
-      <c r="R163" s="42">
-        <v>0</v>
-      </c>
-      <c r="S163" s="42">
-        <v>0</v>
-      </c>
-      <c r="T163" s="41" t="s">
+      <c r="P164" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q164" s="59">
+        <v>0</v>
+      </c>
+      <c r="R164" s="59">
+        <v>0</v>
+      </c>
+      <c r="S164" s="59">
+        <v>0</v>
+      </c>
+      <c r="T164" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="U163" s="41" t="s">
+      <c r="U164" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="V163" s="41" t="s">
+      <c r="V164" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W163" s="41" t="s">
+      <c r="W164" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X163" s="41" t="s">
+      <c r="X164" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y163" s="41" t="s">
+      <c r="Y164" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="164" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D164" s="43">
+    <row r="165" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D165" s="57">
         <v>6</v>
       </c>
-      <c r="E164" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F164" s="42">
+      <c r="E165" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F165" s="59">
         <v>6</v>
       </c>
-      <c r="G164" s="42">
+      <c r="G165" s="59">
         <v>630890</v>
       </c>
-      <c r="H164" s="42">
+      <c r="H165" s="59">
         <v>83526.37</v>
       </c>
-      <c r="I164" s="42">
-        <v>0</v>
-      </c>
-      <c r="J164" s="42">
-        <v>0</v>
-      </c>
-      <c r="K164" s="42">
-        <v>0</v>
-      </c>
-      <c r="L164" s="42">
-        <v>0</v>
-      </c>
-      <c r="M164" s="42">
+      <c r="I165" s="59">
+        <v>0</v>
+      </c>
+      <c r="J165" s="59">
+        <v>0</v>
+      </c>
+      <c r="K165" s="59">
+        <v>0</v>
+      </c>
+      <c r="L165" s="59">
+        <v>0</v>
+      </c>
+      <c r="M165" s="59">
         <v>714416.3</v>
       </c>
-      <c r="N164" s="42">
+      <c r="N165" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O164" s="42">
+      <c r="O165" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P164" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q164" s="42">
-        <v>0</v>
-      </c>
-      <c r="R164" s="42">
-        <v>0</v>
-      </c>
-      <c r="S164" s="42">
-        <v>0</v>
-      </c>
-      <c r="T164" s="41" t="s">
+      <c r="P165" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q165" s="59">
+        <v>0</v>
+      </c>
+      <c r="R165" s="59">
+        <v>0</v>
+      </c>
+      <c r="S165" s="59">
+        <v>0</v>
+      </c>
+      <c r="T165" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="U164" s="41" t="s">
+      <c r="U165" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="V164" s="41" t="s">
+      <c r="V165" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W164" s="41" t="s">
+      <c r="W165" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X164" s="41" t="s">
+      <c r="X165" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y164" s="41" t="s">
+      <c r="Y165" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="165" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D165" s="43">
+    <row r="166" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D166" s="57">
         <v>7</v>
       </c>
-      <c r="E165" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F165" s="42">
+      <c r="E166" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F166" s="59">
         <v>7</v>
       </c>
-      <c r="G165" s="42">
+      <c r="G166" s="59">
         <v>628463</v>
       </c>
-      <c r="H165" s="42">
+      <c r="H166" s="59">
         <v>58136.77</v>
       </c>
-      <c r="I165" s="42">
-        <v>0</v>
-      </c>
-      <c r="J165" s="42">
-        <v>0</v>
-      </c>
-      <c r="K165" s="42">
-        <v>0</v>
-      </c>
-      <c r="L165" s="42">
-        <v>0</v>
-      </c>
-      <c r="M165" s="42">
+      <c r="I166" s="59">
+        <v>0</v>
+      </c>
+      <c r="J166" s="59">
+        <v>0</v>
+      </c>
+      <c r="K166" s="59">
+        <v>0</v>
+      </c>
+      <c r="L166" s="59">
+        <v>0</v>
+      </c>
+      <c r="M166" s="59">
         <v>686599.7</v>
       </c>
-      <c r="N165" s="42">
+      <c r="N166" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O165" s="42">
+      <c r="O166" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P165" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q165" s="42">
-        <v>0</v>
-      </c>
-      <c r="R165" s="42">
-        <v>0</v>
-      </c>
-      <c r="S165" s="42">
-        <v>0</v>
-      </c>
-      <c r="T165" s="41" t="s">
+      <c r="P166" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q166" s="59">
+        <v>0</v>
+      </c>
+      <c r="R166" s="59">
+        <v>0</v>
+      </c>
+      <c r="S166" s="59">
+        <v>0</v>
+      </c>
+      <c r="T166" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="U165" s="41" t="s">
+      <c r="U166" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="V165" s="41" t="s">
+      <c r="V166" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W165" s="41" t="s">
+      <c r="W166" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X165" s="41" t="s">
+      <c r="X166" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y165" s="41" t="s">
+      <c r="Y166" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="166" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D166" s="43">
+    <row r="167" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D167" s="57">
         <v>8</v>
       </c>
-      <c r="E166" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F166" s="42">
+      <c r="E167" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F167" s="59">
         <v>8</v>
       </c>
-      <c r="G166" s="42">
+      <c r="G167" s="59">
         <v>640180.4</v>
       </c>
-      <c r="H166" s="42">
+      <c r="H167" s="59">
         <v>34987.17</v>
       </c>
-      <c r="I166" s="42">
-        <v>0</v>
-      </c>
-      <c r="J166" s="42">
-        <v>0</v>
-      </c>
-      <c r="K166" s="42">
-        <v>0</v>
-      </c>
-      <c r="L166" s="42">
-        <v>0</v>
-      </c>
-      <c r="M166" s="42">
+      <c r="I167" s="59">
+        <v>0</v>
+      </c>
+      <c r="J167" s="59">
+        <v>0</v>
+      </c>
+      <c r="K167" s="59">
+        <v>0</v>
+      </c>
+      <c r="L167" s="59">
+        <v>0</v>
+      </c>
+      <c r="M167" s="59">
         <v>675167.6</v>
       </c>
-      <c r="N166" s="42">
+      <c r="N167" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O166" s="42">
+      <c r="O167" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P166" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q166" s="42">
-        <v>0</v>
-      </c>
-      <c r="R166" s="42">
-        <v>0</v>
-      </c>
-      <c r="S166" s="42">
-        <v>0</v>
-      </c>
-      <c r="T166" s="41" t="s">
+      <c r="P167" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q167" s="59">
+        <v>0</v>
+      </c>
+      <c r="R167" s="59">
+        <v>0</v>
+      </c>
+      <c r="S167" s="59">
+        <v>0</v>
+      </c>
+      <c r="T167" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="U166" s="41" t="s">
+      <c r="U167" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="V166" s="41" t="s">
+      <c r="V167" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W166" s="41" t="s">
+      <c r="W167" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X166" s="41" t="s">
+      <c r="X167" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y166" s="41" t="s">
+      <c r="Y167" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="167" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D167" s="43">
+    <row r="168" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D168" s="57">
         <v>9</v>
       </c>
-      <c r="E167" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F167" s="42">
+      <c r="E168" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F168" s="59">
         <v>9</v>
       </c>
-      <c r="G167" s="42">
+      <c r="G168" s="59">
         <v>779809</v>
       </c>
-      <c r="H167" s="42">
+      <c r="H168" s="59">
         <v>73838.87</v>
       </c>
-      <c r="I167" s="42">
-        <v>0</v>
-      </c>
-      <c r="J167" s="42">
-        <v>0</v>
-      </c>
-      <c r="K167" s="42">
-        <v>0</v>
-      </c>
-      <c r="L167" s="42">
-        <v>0</v>
-      </c>
-      <c r="M167" s="42">
+      <c r="I168" s="59">
+        <v>0</v>
+      </c>
+      <c r="J168" s="59">
+        <v>0</v>
+      </c>
+      <c r="K168" s="59">
+        <v>0</v>
+      </c>
+      <c r="L168" s="59">
+        <v>0</v>
+      </c>
+      <c r="M168" s="59">
         <v>853647.9</v>
       </c>
-      <c r="N167" s="42">
+      <c r="N168" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O167" s="42">
+      <c r="O168" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P167" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q167" s="42">
-        <v>0</v>
-      </c>
-      <c r="R167" s="42">
-        <v>0</v>
-      </c>
-      <c r="S167" s="42">
-        <v>0</v>
-      </c>
-      <c r="T167" s="41" t="s">
+      <c r="P168" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q168" s="59">
+        <v>0</v>
+      </c>
+      <c r="R168" s="59">
+        <v>0</v>
+      </c>
+      <c r="S168" s="59">
+        <v>0</v>
+      </c>
+      <c r="T168" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="U167" s="41" t="s">
+      <c r="U168" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="V167" s="41" t="s">
+      <c r="V168" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W167" s="41" t="s">
+      <c r="W168" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X167" s="41" t="s">
+      <c r="X168" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y167" s="41" t="s">
+      <c r="Y168" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="168" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D168" s="43">
+    <row r="169" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D169" s="57">
         <v>10</v>
       </c>
-      <c r="E168" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F168" s="42">
+      <c r="E169" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F169" s="59">
         <v>10</v>
       </c>
-      <c r="G168" s="42">
+      <c r="G169" s="59">
         <v>697763.8</v>
       </c>
-      <c r="H168" s="42">
+      <c r="H169" s="59">
         <v>26133.33</v>
       </c>
-      <c r="I168" s="42">
-        <v>0</v>
-      </c>
-      <c r="J168" s="42">
-        <v>0</v>
-      </c>
-      <c r="K168" s="42">
-        <v>0</v>
-      </c>
-      <c r="L168" s="42">
-        <v>0</v>
-      </c>
-      <c r="M168" s="42">
+      <c r="I169" s="59">
+        <v>0</v>
+      </c>
+      <c r="J169" s="59">
+        <v>0</v>
+      </c>
+      <c r="K169" s="59">
+        <v>0</v>
+      </c>
+      <c r="L169" s="59">
+        <v>0</v>
+      </c>
+      <c r="M169" s="59">
         <v>723897.1</v>
       </c>
-      <c r="N168" s="42">
+      <c r="N169" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O168" s="42">
+      <c r="O169" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P168" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q168" s="42">
-        <v>0</v>
-      </c>
-      <c r="R168" s="42">
-        <v>0</v>
-      </c>
-      <c r="S168" s="42">
-        <v>0</v>
-      </c>
-      <c r="T168" s="41" t="s">
+      <c r="P169" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q169" s="59">
+        <v>0</v>
+      </c>
+      <c r="R169" s="59">
+        <v>0</v>
+      </c>
+      <c r="S169" s="59">
+        <v>0</v>
+      </c>
+      <c r="T169" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U168" s="41" t="s">
+      <c r="U169" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="V168" s="41" t="s">
+      <c r="V169" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W168" s="41" t="s">
+      <c r="W169" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X168" s="41" t="s">
+      <c r="X169" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y168" s="41" t="s">
+      <c r="Y169" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="169" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D169" s="43">
+    <row r="170" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D170" s="57">
         <v>11</v>
       </c>
-      <c r="E169" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F169" s="42">
+      <c r="E170" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F170" s="59">
         <v>11</v>
       </c>
-      <c r="G169" s="42">
+      <c r="G170" s="59">
         <v>586706.9</v>
       </c>
-      <c r="H169" s="42">
+      <c r="H170" s="59">
         <v>65078.27</v>
       </c>
-      <c r="I169" s="42">
-        <v>0</v>
-      </c>
-      <c r="J169" s="42">
-        <v>0</v>
-      </c>
-      <c r="K169" s="42">
-        <v>0</v>
-      </c>
-      <c r="L169" s="42">
-        <v>0</v>
-      </c>
-      <c r="M169" s="42">
+      <c r="I170" s="59">
+        <v>0</v>
+      </c>
+      <c r="J170" s="59">
+        <v>0</v>
+      </c>
+      <c r="K170" s="59">
+        <v>0</v>
+      </c>
+      <c r="L170" s="59">
+        <v>0</v>
+      </c>
+      <c r="M170" s="59">
         <v>651785.19999999995</v>
       </c>
-      <c r="N169" s="42">
+      <c r="N170" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O169" s="42">
+      <c r="O170" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P169" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q169" s="42">
-        <v>0</v>
-      </c>
-      <c r="R169" s="42">
-        <v>0</v>
-      </c>
-      <c r="S169" s="42">
-        <v>0</v>
-      </c>
-      <c r="T169" s="41" t="s">
+      <c r="P170" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q170" s="59">
+        <v>0</v>
+      </c>
+      <c r="R170" s="59">
+        <v>0</v>
+      </c>
+      <c r="S170" s="59">
+        <v>0</v>
+      </c>
+      <c r="T170" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="U169" s="41" t="s">
+      <c r="U170" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V169" s="41" t="s">
+      <c r="V170" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W169" s="41" t="s">
+      <c r="W170" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X169" s="41" t="s">
+      <c r="X170" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y169" s="41" t="s">
+      <c r="Y170" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="170" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D170" s="43">
+    <row r="171" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D171" s="57">
         <v>12</v>
       </c>
-      <c r="E170" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F170" s="42">
+      <c r="E171" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F171" s="59">
         <v>12</v>
       </c>
-      <c r="G170" s="42">
+      <c r="G171" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="H170" s="42">
+      <c r="H171" s="59">
         <v>156266.53</v>
       </c>
-      <c r="I170" s="42">
-        <v>0</v>
-      </c>
-      <c r="J170" s="42">
-        <v>0</v>
-      </c>
-      <c r="K170" s="42">
-        <v>0</v>
-      </c>
-      <c r="L170" s="42">
-        <v>0</v>
-      </c>
-      <c r="M170" s="42">
+      <c r="I171" s="59">
+        <v>0</v>
+      </c>
+      <c r="J171" s="59">
+        <v>0</v>
+      </c>
+      <c r="K171" s="59">
+        <v>0</v>
+      </c>
+      <c r="L171" s="59">
+        <v>0</v>
+      </c>
+      <c r="M171" s="59">
         <v>731696.8</v>
       </c>
-      <c r="N170" s="42">
+      <c r="N171" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="O170" s="42">
+      <c r="O171" s="59">
         <v>26133.33</v>
       </c>
-      <c r="P170" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q170" s="42">
-        <v>0</v>
-      </c>
-      <c r="R170" s="42">
-        <v>0</v>
-      </c>
-      <c r="S170" s="42">
-        <v>0</v>
-      </c>
-      <c r="T170" s="41" t="s">
+      <c r="P171" s="59">
+        <v>0</v>
+      </c>
+      <c r="Q171" s="59">
+        <v>0</v>
+      </c>
+      <c r="R171" s="59">
+        <v>0</v>
+      </c>
+      <c r="S171" s="59">
+        <v>0</v>
+      </c>
+      <c r="T171" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="U170" s="41" t="s">
+      <c r="U171" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="V170" s="41" t="s">
+      <c r="V171" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="W170" s="41" t="s">
+      <c r="W171" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="X170" s="41" t="s">
+      <c r="X171" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="Y170" s="41" t="s">
+      <c r="Y171" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="171" spans="4:25" x14ac:dyDescent="0.35">
-      <c r="D171" s="57"/>
-      <c r="E171" s="58"/>
-      <c r="F171" s="59"/>
-      <c r="G171" s="60">
-        <f>SUM(G159:G170)</f>
+    <row r="172" spans="4:25" s="60" customFormat="1" ht="16" x14ac:dyDescent="0.3">
+      <c r="D172" s="61"/>
+      <c r="E172" s="62"/>
+      <c r="F172" s="63"/>
+      <c r="G172" s="65">
+        <f>SUM(G160:G171)</f>
         <v>7891121.8000000007</v>
       </c>
-      <c r="H171" s="59"/>
-      <c r="I171" s="59"/>
-      <c r="J171" s="59"/>
-      <c r="K171" s="59"/>
-      <c r="L171" s="59"/>
-      <c r="M171" s="59"/>
-      <c r="N171" s="59"/>
-      <c r="O171" s="59"/>
-      <c r="P171" s="59"/>
-      <c r="Q171" s="59"/>
-      <c r="R171" s="59"/>
-      <c r="S171" s="59"/>
-      <c r="T171" s="58"/>
-      <c r="U171" s="58"/>
-      <c r="V171" s="58"/>
-      <c r="W171" s="58"/>
-      <c r="X171" s="58"/>
-      <c r="Y171" s="58"/>
-    </row>
-    <row r="174" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D174" s="43">
-        <v>1</v>
-      </c>
-      <c r="E174" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F174" s="42">
+      <c r="H172" s="65">
+        <f>SUM(H160:H171)</f>
+        <v>1547396.0500000005</v>
+      </c>
+      <c r="I172" s="63"/>
+      <c r="J172" s="63"/>
+      <c r="K172" s="63"/>
+      <c r="L172" s="63"/>
+      <c r="M172" s="65">
+        <f>SUM(M160:M171)</f>
+        <v>9438517.9000000004</v>
+      </c>
+      <c r="N172" s="65">
+        <f>SUM(N160:N171)</f>
+        <v>6905162.4000000013</v>
+      </c>
+      <c r="O172" s="65">
+        <f>SUM(O160:O171)</f>
+        <v>313599.96000000008</v>
+      </c>
+      <c r="P172" s="63"/>
+      <c r="Q172" s="63"/>
+      <c r="R172" s="63"/>
+      <c r="S172" s="63"/>
+      <c r="T172" s="62"/>
+      <c r="U172" s="62"/>
+      <c r="V172" s="62"/>
+      <c r="W172" s="62"/>
+      <c r="X172" s="62"/>
+      <c r="Y172" s="62"/>
+    </row>
+    <row r="174" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D174" s="17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="175" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D175" s="57">
+        <v>1</v>
+      </c>
+      <c r="E175" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F175" s="59">
         <v>1173418.8999999999</v>
       </c>
-      <c r="G174" s="42">
-        <v>0</v>
-      </c>
-      <c r="H174" s="42">
+      <c r="G175" s="59">
+        <v>0</v>
+      </c>
+      <c r="H175" s="59">
         <v>4010745.6</v>
       </c>
-      <c r="I174" s="42">
+      <c r="I175" s="59">
         <v>521241.27</v>
       </c>
-      <c r="J174" s="42">
-        <v>0</v>
-      </c>
-      <c r="K174" s="42">
-        <v>0</v>
-      </c>
-      <c r="L174" s="42">
-        <v>0</v>
-      </c>
-      <c r="M174" s="42">
-        <v>0</v>
-      </c>
-      <c r="N174" s="41" t="s">
+      <c r="J175" s="59">
+        <v>0</v>
+      </c>
+      <c r="K175" s="59">
+        <v>0</v>
+      </c>
+      <c r="L175" s="59">
+        <v>0</v>
+      </c>
+      <c r="M175" s="59">
+        <v>0</v>
+      </c>
+      <c r="N175" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="O174" s="41" t="s">
+      <c r="O175" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="P174" s="41" t="s">
+      <c r="P175" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="Q174" s="41" t="s">
+      <c r="Q175" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="R174" s="41" t="s">
+      <c r="R175" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="S174" s="41" t="s">
+      <c r="S175" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="175" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D175" s="43">
+    <row r="176" spans="4:25" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D176" s="57">
         <v>2</v>
       </c>
-      <c r="E175" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F175" s="42">
+      <c r="E176" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F176" s="59">
         <v>168352.9</v>
       </c>
-      <c r="G175" s="42">
-        <v>0</v>
-      </c>
-      <c r="H175" s="42">
+      <c r="G176" s="59">
+        <v>0</v>
+      </c>
+      <c r="H176" s="59">
         <v>575430.19999999995</v>
       </c>
-      <c r="I175" s="42">
+      <c r="I176" s="59">
         <v>156266.53</v>
       </c>
-      <c r="J175" s="42">
-        <v>0</v>
-      </c>
-      <c r="K175" s="42">
-        <v>0</v>
-      </c>
-      <c r="L175" s="42">
-        <v>0</v>
-      </c>
-      <c r="M175" s="42">
-        <v>0</v>
-      </c>
-      <c r="N175" s="41" t="s">
+      <c r="J176" s="59">
+        <v>0</v>
+      </c>
+      <c r="K176" s="59">
+        <v>0</v>
+      </c>
+      <c r="L176" s="59">
+        <v>0</v>
+      </c>
+      <c r="M176" s="59">
+        <v>0</v>
+      </c>
+      <c r="N176" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="O175" s="41" t="s">
+      <c r="O176" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="P175" s="41" t="s">
+      <c r="P176" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="Q175" s="41" t="s">
+      <c r="Q176" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="R175" s="41" t="s">
+      <c r="R176" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="S175" s="41" t="s">
+      <c r="S176" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="176" spans="4:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D176" s="43">
+    <row r="177" spans="4:26" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D177" s="57">
         <v>3</v>
       </c>
-      <c r="E176" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F176" s="42">
+      <c r="E177" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F177" s="59">
         <v>762780.1</v>
       </c>
-      <c r="G176" s="42">
-        <v>0</v>
-      </c>
-      <c r="H176" s="42">
+      <c r="G177" s="59">
+        <v>0</v>
+      </c>
+      <c r="H177" s="59">
         <v>2607182.2000000002</v>
       </c>
-      <c r="I176" s="42">
+      <c r="I177" s="59">
         <v>843754.9</v>
       </c>
-      <c r="J176" s="42">
-        <v>0</v>
-      </c>
-      <c r="K176" s="42">
-        <v>0</v>
-      </c>
-      <c r="L176" s="42">
-        <v>0</v>
-      </c>
-      <c r="M176" s="42">
-        <v>0</v>
-      </c>
-      <c r="N176" s="41" t="s">
+      <c r="J177" s="59">
+        <v>0</v>
+      </c>
+      <c r="K177" s="59">
+        <v>0</v>
+      </c>
+      <c r="L177" s="59">
+        <v>0</v>
+      </c>
+      <c r="M177" s="59">
+        <v>0</v>
+      </c>
+      <c r="N177" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="O176" s="41" t="s">
+      <c r="O177" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="P176" s="41" t="s">
+      <c r="P177" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="Q176" s="41" t="s">
+      <c r="Q177" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="R176" s="41" t="s">
+      <c r="R177" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="S176" s="41" t="s">
+      <c r="S177" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="177" spans="4:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D177" s="43">
+    <row r="178" spans="4:26" s="60" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D178" s="57">
         <v>4</v>
       </c>
-      <c r="E177" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F177" s="42">
+      <c r="E178" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F178" s="59">
         <v>204143.9</v>
       </c>
-      <c r="G177" s="42">
-        <v>0</v>
-      </c>
-      <c r="H177" s="42">
+      <c r="G178" s="59">
+        <v>0</v>
+      </c>
+      <c r="H178" s="59">
         <v>697763.8</v>
       </c>
-      <c r="I177" s="42">
+      <c r="I178" s="59">
         <v>26133.33</v>
       </c>
-      <c r="J177" s="42">
-        <v>0</v>
-      </c>
-      <c r="K177" s="42">
-        <v>0</v>
-      </c>
-      <c r="L177" s="42">
-        <v>0</v>
-      </c>
-      <c r="M177" s="42">
-        <v>0</v>
-      </c>
-      <c r="N177" s="41" t="s">
+      <c r="J178" s="59">
+        <v>0</v>
+      </c>
+      <c r="K178" s="59">
+        <v>0</v>
+      </c>
+      <c r="L178" s="59">
+        <v>0</v>
+      </c>
+      <c r="M178" s="59">
+        <v>0</v>
+      </c>
+      <c r="N178" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="O177" s="41" t="s">
+      <c r="O178" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="P177" s="41" t="s">
+      <c r="P178" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="Q177" s="41" t="s">
+      <c r="Q178" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="R177" s="41" t="s">
+      <c r="R178" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="S177" s="41" t="s">
+      <c r="S178" s="58" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="178" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="F178" s="56">
-        <f>SUM(F174:F177)</f>
+    <row r="179" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="F179" s="56">
+        <f>SUM(F175:F178)</f>
         <v>2308695.7999999998</v>
       </c>
-      <c r="H178">
-        <f>SUM(H174:H177)</f>
+      <c r="H179">
+        <f>SUM(H175:H178)</f>
         <v>7891121.7999999998</v>
       </c>
-    </row>
-    <row r="181" spans="4:19" x14ac:dyDescent="0.35">
-      <c r="G181">
-        <f>G171/F178</f>
+      <c r="I179">
+        <f>SUM(I175:I178)</f>
+        <v>1547396.0300000003</v>
+      </c>
+    </row>
+    <row r="182" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="G182">
+        <f>G172/F179</f>
         <v>3.4179998075103706</v>
       </c>
-      <c r="H181">
+      <c r="H182">
         <f>4010745.6+575430.2+3304946</f>
         <v>7891121.7999999998</v>
+      </c>
+    </row>
+    <row r="183" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="H183" s="64">
+        <f>H182-G172</f>
+        <v>0</v>
+      </c>
+      <c r="I183" s="64">
+        <f>I179-H172</f>
+        <v>-2.0000000251457095E-2</v>
+      </c>
+    </row>
+    <row r="186" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="D186" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="187" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="D187" s="66">
+        <v>1</v>
+      </c>
+      <c r="E187" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F187" s="68">
+        <v>1173418.8999999999</v>
+      </c>
+      <c r="G187" s="68">
+        <v>0</v>
+      </c>
+      <c r="H187" s="68">
+        <v>4010745.6</v>
+      </c>
+      <c r="I187" s="68">
+        <v>521241.27</v>
+      </c>
+      <c r="J187" s="68">
+        <v>0</v>
+      </c>
+      <c r="K187" s="68">
+        <v>0</v>
+      </c>
+      <c r="L187" s="68">
+        <v>0</v>
+      </c>
+      <c r="M187" s="68">
+        <v>0</v>
+      </c>
+      <c r="N187" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="O187" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="P187" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q187" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R187" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S187" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T187" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U187" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V187" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W187" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X187" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y187" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z187" s="69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="D188" s="66">
+        <v>2</v>
+      </c>
+      <c r="E188" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F188" s="68">
+        <v>168352.9</v>
+      </c>
+      <c r="G188" s="68">
+        <v>0</v>
+      </c>
+      <c r="H188" s="68">
+        <v>575430.19999999995</v>
+      </c>
+      <c r="I188" s="68">
+        <v>156266.53</v>
+      </c>
+      <c r="J188" s="68">
+        <v>0</v>
+      </c>
+      <c r="K188" s="68">
+        <v>0</v>
+      </c>
+      <c r="L188" s="68">
+        <v>0</v>
+      </c>
+      <c r="M188" s="68">
+        <v>0</v>
+      </c>
+      <c r="N188" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="O188" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="P188" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q188" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R188" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S188" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T188" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U188" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V188" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W188" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X188" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y188" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z188" s="69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="D189" s="66">
+        <v>3</v>
+      </c>
+      <c r="E189" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F189" s="68">
+        <v>762780.1</v>
+      </c>
+      <c r="G189" s="68">
+        <v>0</v>
+      </c>
+      <c r="H189" s="68">
+        <v>2607182.2000000002</v>
+      </c>
+      <c r="I189" s="68">
+        <v>843754.9</v>
+      </c>
+      <c r="J189" s="68">
+        <v>0</v>
+      </c>
+      <c r="K189" s="68">
+        <v>0</v>
+      </c>
+      <c r="L189" s="68">
+        <v>0</v>
+      </c>
+      <c r="M189" s="68">
+        <v>0</v>
+      </c>
+      <c r="N189" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="O189" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="P189" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q189" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R189" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S189" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T189" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U189" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V189" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W189" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X189" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y189" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z189" s="69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="4:26" x14ac:dyDescent="0.35">
+      <c r="D190" s="66">
+        <v>4</v>
+      </c>
+      <c r="E190" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F190" s="68">
+        <v>204143.9</v>
+      </c>
+      <c r="G190" s="68">
+        <v>0</v>
+      </c>
+      <c r="H190" s="68">
+        <v>697763.8</v>
+      </c>
+      <c r="I190" s="68">
+        <v>26133.33</v>
+      </c>
+      <c r="J190" s="68">
+        <v>0</v>
+      </c>
+      <c r="K190" s="68">
+        <v>0</v>
+      </c>
+      <c r="L190" s="68">
+        <v>0</v>
+      </c>
+      <c r="M190" s="68">
+        <v>0</v>
+      </c>
+      <c r="N190" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="O190" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="P190" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q190" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R190" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S190" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T190" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U190" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V190" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W190" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X190" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y190" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z190" s="69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D193" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="194" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D194" s="66">
+        <v>1</v>
+      </c>
+      <c r="E194" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F194" s="68">
+        <v>1173418.8999999999</v>
+      </c>
+      <c r="G194" s="68">
+        <v>0</v>
+      </c>
+      <c r="H194" s="68">
+        <v>4010745.6</v>
+      </c>
+      <c r="I194" s="68">
+        <v>521241.27</v>
+      </c>
+      <c r="J194" s="68">
+        <v>0</v>
+      </c>
+      <c r="K194" s="68">
+        <v>0</v>
+      </c>
+      <c r="L194" s="68">
+        <v>0</v>
+      </c>
+      <c r="M194" s="68">
+        <v>0</v>
+      </c>
+      <c r="N194" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="O194" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="P194" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q194" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R194" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S194" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T194" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U194" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V194" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W194" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X194" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y194" s="67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="195" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D195" s="66">
+        <v>2</v>
+      </c>
+      <c r="E195" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F195" s="68">
+        <v>168352.9</v>
+      </c>
+      <c r="G195" s="68">
+        <v>0</v>
+      </c>
+      <c r="H195" s="68">
+        <v>575430.19999999995</v>
+      </c>
+      <c r="I195" s="68">
+        <v>156266.53</v>
+      </c>
+      <c r="J195" s="68">
+        <v>0</v>
+      </c>
+      <c r="K195" s="68">
+        <v>0</v>
+      </c>
+      <c r="L195" s="68">
+        <v>0</v>
+      </c>
+      <c r="M195" s="68">
+        <v>0</v>
+      </c>
+      <c r="N195" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="O195" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="P195" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q195" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R195" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S195" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T195" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U195" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V195" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W195" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X195" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y195" s="67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="196" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D196" s="66">
+        <v>3</v>
+      </c>
+      <c r="E196" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F196" s="68">
+        <v>762780.1</v>
+      </c>
+      <c r="G196" s="68">
+        <v>0</v>
+      </c>
+      <c r="H196" s="68">
+        <v>2607182.2000000002</v>
+      </c>
+      <c r="I196" s="68">
+        <v>843754.9</v>
+      </c>
+      <c r="J196" s="68">
+        <v>0</v>
+      </c>
+      <c r="K196" s="68">
+        <v>0</v>
+      </c>
+      <c r="L196" s="68">
+        <v>0</v>
+      </c>
+      <c r="M196" s="68">
+        <v>0</v>
+      </c>
+      <c r="N196" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="O196" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="P196" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q196" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R196" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S196" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T196" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U196" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V196" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W196" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X196" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y196" s="67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="197" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D197" s="66">
+        <v>4</v>
+      </c>
+      <c r="E197" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="F197" s="68">
+        <v>204143.9</v>
+      </c>
+      <c r="G197" s="68">
+        <v>0</v>
+      </c>
+      <c r="H197" s="68">
+        <v>697763.8</v>
+      </c>
+      <c r="I197" s="68">
+        <v>26133.33</v>
+      </c>
+      <c r="J197" s="68">
+        <v>0</v>
+      </c>
+      <c r="K197" s="68">
+        <v>0</v>
+      </c>
+      <c r="L197" s="68">
+        <v>0</v>
+      </c>
+      <c r="M197" s="68">
+        <v>0</v>
+      </c>
+      <c r="N197" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="O197" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="P197" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q197" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="R197" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="S197" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="T197" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="U197" s="68">
+        <v>303429</v>
+      </c>
+      <c r="V197" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="W197" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="X197" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y197" s="67" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="200" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D200" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="201" spans="4:25" x14ac:dyDescent="0.35">
+      <c r="D201" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check of savings measures table
</commit_message>
<xml_diff>
--- a/data/TEST_Values_Tables.xlsx
+++ b/data/TEST_Values_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tishmanspeyercloud-my.sharepoint.com/personal/prode_tishmanspeyer_com/Documents/Documents/R/NCZ_Interventions/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{35015F2C-5694-4A86-B3A9-A4D61B86BB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92B27F87-7789-4455-876A-7F2A99A1969D}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{35015F2C-5694-4A86-B3A9-A4D61B86BB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70FCCBE0-91BD-4E71-8000-5D1EC2E76B83}"/>
   <bookViews>
-    <workbookView xWindow="730" yWindow="3050" windowWidth="20510" windowHeight="10540" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
+    <workbookView xWindow="-1860" yWindow="2010" windowWidth="16920" windowHeight="9320" xr2:uid="{5E605C51-9C84-4C57-AB33-34EB38F96990}"/>
   </bookViews>
   <sheets>
     <sheet name="R" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="167">
   <si>
     <t>160 Spear</t>
   </si>
@@ -442,6 +442,105 @@
   </si>
   <si>
     <t>UP TO 230</t>
+  </si>
+  <si>
+    <t>Savings Measures</t>
+  </si>
+  <si>
+    <t>Retrocommissioning  (RCx)</t>
+  </si>
+  <si>
+    <t>Heating &amp; Cooling &amp; Base</t>
+  </si>
+  <si>
+    <t>Complete BMS commissioning</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Façade air stopping</t>
+  </si>
+  <si>
+    <t>Heating &amp; Cooling</t>
+  </si>
+  <si>
+    <t>caulking and general air stopping</t>
+  </si>
+  <si>
+    <t>New High Efficiency Windows</t>
+  </si>
+  <si>
+    <t>New Windows tripple pane R6@30SHG</t>
+  </si>
+  <si>
+    <t>New Electric Chillers</t>
+  </si>
+  <si>
+    <t>Chiller Plant</t>
+  </si>
+  <si>
+    <t>Pneumatic Converstion</t>
+  </si>
+  <si>
+    <t>BMS Expansion</t>
+  </si>
+  <si>
+    <t>Elevator energy revovery</t>
+  </si>
+  <si>
+    <t>Optional add to elevator package</t>
+  </si>
+  <si>
+    <t>sqft</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>base loads</t>
+  </si>
+  <si>
+    <t>cooling loads</t>
+  </si>
+  <si>
+    <t>heating loads</t>
+  </si>
+  <si>
+    <t>intervention name</t>
+  </si>
+  <si>
+    <t>savings</t>
+  </si>
+  <si>
+    <t>orider</t>
+  </si>
+  <si>
+    <t>description of measure</t>
+  </si>
+  <si>
+    <t>change in Elect</t>
+  </si>
+  <si>
+    <t>Change in Ngas</t>
+  </si>
+  <si>
+    <t>Change in Steam</t>
+  </si>
+  <si>
+    <t>saved base</t>
+  </si>
+  <si>
+    <t>saved cooling</t>
+  </si>
+  <si>
+    <t>saved heating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabled formed after line 510 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">heating 2 lines above added together. </t>
   </si>
 </sst>
 </file>
@@ -798,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -969,6 +1068,7 @@
     <xf numFmtId="43" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1036,14 +1136,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1081,7 +1177,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1187,7 +1283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1329,7 +1425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1337,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3813FFD9-5E5D-46D2-877D-6E8E65729695}">
-  <dimension ref="C1:Z218"/>
+  <dimension ref="A1:Z236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="126" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D214" sqref="D214"/>
+    <sheetView tabSelected="1" topLeftCell="J210" zoomScale="126" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J224" sqref="J224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,6 +1452,8 @@
     <col min="13" max="13" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.36328125" customWidth="1"/>
     <col min="15" max="15" width="21.7265625" customWidth="1"/>
+    <col min="16" max="16" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:15" x14ac:dyDescent="0.35">
@@ -6966,7 +7064,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C209" s="70">
         <v>58</v>
       </c>
@@ -6980,23 +7078,25 @@
         <v>91</v>
       </c>
     </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
       <c r="E210" s="73">
         <f>SUM(E206:E209)</f>
         <v>7891121.7999999998</v>
       </c>
     </row>
-    <row r="213" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="212" spans="1:17" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="213" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="D213" s="17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="214" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="D214" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="215" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:17" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C215" s="70">
         <v>1</v>
       </c>
@@ -7010,7 +7110,7 @@
         <v>521241.27</v>
       </c>
     </row>
-    <row r="216" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:17" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C216" s="70">
         <v>2</v>
       </c>
@@ -7024,7 +7124,7 @@
         <v>1000021.43</v>
       </c>
     </row>
-    <row r="217" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:17" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C217" s="70">
         <v>3</v>
       </c>
@@ -7038,10 +7138,718 @@
         <v>26133.33</v>
       </c>
     </row>
-    <row r="218" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="F218" s="75">
         <f>SUM(F215:F217)</f>
         <v>1547396.0300000003</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="221" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="E221" s="74">
+        <f>E209+E208</f>
+        <v>3304946</v>
+      </c>
+      <c r="F221" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A222" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B224" t="s">
+        <v>98</v>
+      </c>
+      <c r="C224" t="s">
+        <v>150</v>
+      </c>
+      <c r="D224" t="s">
+        <v>151</v>
+      </c>
+      <c r="E224" t="s">
+        <v>152</v>
+      </c>
+      <c r="F224" t="s">
+        <v>153</v>
+      </c>
+      <c r="G224" t="s">
+        <v>154</v>
+      </c>
+      <c r="H224" t="s">
+        <v>155</v>
+      </c>
+      <c r="I224" t="s">
+        <v>156</v>
+      </c>
+      <c r="J224" t="s">
+        <v>157</v>
+      </c>
+      <c r="K224" t="s">
+        <v>158</v>
+      </c>
+      <c r="L224" t="s">
+        <v>159</v>
+      </c>
+      <c r="M224" t="s">
+        <v>160</v>
+      </c>
+      <c r="N224" t="s">
+        <v>161</v>
+      </c>
+      <c r="O224" t="s">
+        <v>162</v>
+      </c>
+      <c r="P224" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q224" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="225" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A225" s="43">
+        <v>1</v>
+      </c>
+      <c r="B225" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C225" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D225" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E225" s="42">
+        <v>26133.33</v>
+      </c>
+      <c r="F225" s="42">
+        <v>521241.3</v>
+      </c>
+      <c r="G225" s="42">
+        <v>1000021.4</v>
+      </c>
+      <c r="H225" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="I225" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="J225" s="42">
+        <v>1</v>
+      </c>
+      <c r="K225" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="L225" s="42">
+        <v>0.04</v>
+      </c>
+      <c r="M225" s="42">
+        <v>0.04</v>
+      </c>
+      <c r="N225" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O225" s="42">
+        <v>1045.3330000000001</v>
+      </c>
+      <c r="P225" s="42">
+        <v>20849.651000000002</v>
+      </c>
+      <c r="Q225" s="42">
+        <v>40000.86</v>
+      </c>
+      <c r="R225" s="76"/>
+    </row>
+    <row r="226" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A226" s="43">
+        <v>2</v>
+      </c>
+      <c r="B226" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C226" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D226" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E226" s="42">
+        <v>25088</v>
+      </c>
+      <c r="F226" s="42">
+        <v>500391.6</v>
+      </c>
+      <c r="G226" s="42">
+        <v>960020.6</v>
+      </c>
+      <c r="H226" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="I226" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="J226" s="42">
+        <v>3</v>
+      </c>
+      <c r="K226" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="L226" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="M226" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="N226" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O226" s="42">
+        <v>0</v>
+      </c>
+      <c r="P226" s="42">
+        <v>10007.832</v>
+      </c>
+      <c r="Q226" s="42">
+        <v>19200.41</v>
+      </c>
+    </row>
+    <row r="227" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A227" s="43">
+        <v>3</v>
+      </c>
+      <c r="B227" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C227" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D227" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E227" s="42">
+        <v>25088</v>
+      </c>
+      <c r="F227" s="42">
+        <v>490383.8</v>
+      </c>
+      <c r="G227" s="42">
+        <v>940820.2</v>
+      </c>
+      <c r="H227" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="I227" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="J227" s="42">
+        <v>4</v>
+      </c>
+      <c r="K227" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="L227" s="42">
+        <v>0.05</v>
+      </c>
+      <c r="M227" s="42">
+        <v>0.05</v>
+      </c>
+      <c r="N227" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O227" s="42">
+        <v>0</v>
+      </c>
+      <c r="P227" s="42">
+        <v>24519.188999999998</v>
+      </c>
+      <c r="Q227" s="42">
+        <v>47041.01</v>
+      </c>
+    </row>
+    <row r="228" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A228" s="43">
+        <v>4</v>
+      </c>
+      <c r="B228" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C228" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D228" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E228" s="42">
+        <v>25088</v>
+      </c>
+      <c r="F228" s="42">
+        <v>465864.6</v>
+      </c>
+      <c r="G228" s="42">
+        <v>893779.2</v>
+      </c>
+      <c r="H228" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I228" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="J228" s="42">
+        <v>5</v>
+      </c>
+      <c r="K228" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="L228" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="M228" s="42">
+        <v>0</v>
+      </c>
+      <c r="N228" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O228" s="42">
+        <v>0</v>
+      </c>
+      <c r="P228" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q228" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A229" s="43">
+        <v>5</v>
+      </c>
+      <c r="B229" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C229" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D229" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E229" s="42">
+        <v>25088</v>
+      </c>
+      <c r="F229" s="42">
+        <v>465864.6</v>
+      </c>
+      <c r="G229" s="42">
+        <v>893779.2</v>
+      </c>
+      <c r="H229" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="I229" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="J229" s="42">
+        <v>6</v>
+      </c>
+      <c r="K229" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="L229" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="M229" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="N229" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O229" s="42">
+        <v>0</v>
+      </c>
+      <c r="P229" s="42">
+        <v>9317.2919999999995</v>
+      </c>
+      <c r="Q229" s="42">
+        <v>17875.580000000002</v>
+      </c>
+    </row>
+    <row r="230" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A230" s="43">
+        <v>6</v>
+      </c>
+      <c r="B230" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C230" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D230" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E230" s="42">
+        <v>25088</v>
+      </c>
+      <c r="F230" s="42">
+        <v>456547.3</v>
+      </c>
+      <c r="G230" s="42">
+        <v>875903.6</v>
+      </c>
+      <c r="H230" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="I230" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="J230" s="42">
+        <v>7</v>
+      </c>
+      <c r="K230" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="L230" s="42">
+        <v>0.01</v>
+      </c>
+      <c r="M230" s="42">
+        <v>0</v>
+      </c>
+      <c r="N230" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O230" s="42">
+        <v>0</v>
+      </c>
+      <c r="P230" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q230" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A231" s="43">
+        <v>7</v>
+      </c>
+      <c r="B231" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C231" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D231" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E231" s="42">
+        <v>575430.23</v>
+      </c>
+      <c r="F231" s="42">
+        <v>4010745.6</v>
+      </c>
+      <c r="G231" s="42">
+        <v>3304946</v>
+      </c>
+      <c r="H231" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="I231" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="J231" s="42">
+        <v>1</v>
+      </c>
+      <c r="K231" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="L231" s="42">
+        <v>0.04</v>
+      </c>
+      <c r="M231" s="42">
+        <v>0.04</v>
+      </c>
+      <c r="N231" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O231" s="42">
+        <v>23017.208999999999</v>
+      </c>
+      <c r="P231" s="42">
+        <v>160429.82500000001</v>
+      </c>
+      <c r="Q231" s="42">
+        <v>132197.84</v>
+      </c>
+    </row>
+    <row r="232" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A232" s="43">
+        <v>8</v>
+      </c>
+      <c r="B232" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C232" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D232" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E232" s="42">
+        <v>552413.02</v>
+      </c>
+      <c r="F232" s="42">
+        <v>3850315.8</v>
+      </c>
+      <c r="G232" s="42">
+        <v>3172748.2</v>
+      </c>
+      <c r="H232" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="I232" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="J232" s="42">
+        <v>3</v>
+      </c>
+      <c r="K232" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="L232" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="M232" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="N232" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O232" s="42">
+        <v>0</v>
+      </c>
+      <c r="P232" s="42">
+        <v>77006.316000000006</v>
+      </c>
+      <c r="Q232" s="42">
+        <v>63454.96</v>
+      </c>
+    </row>
+    <row r="233" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A233" s="43">
+        <v>9</v>
+      </c>
+      <c r="B233" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C233" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D233" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E233" s="42">
+        <v>552413.02</v>
+      </c>
+      <c r="F233" s="42">
+        <v>3773309.5</v>
+      </c>
+      <c r="G233" s="42">
+        <v>3109293.2</v>
+      </c>
+      <c r="H233" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="I233" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="J233" s="42">
+        <v>4</v>
+      </c>
+      <c r="K233" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="L233" s="42">
+        <v>0.05</v>
+      </c>
+      <c r="M233" s="42">
+        <v>0.05</v>
+      </c>
+      <c r="N233" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O233" s="42">
+        <v>0</v>
+      </c>
+      <c r="P233" s="42">
+        <v>188665.47500000001</v>
+      </c>
+      <c r="Q233" s="42">
+        <v>155464.66</v>
+      </c>
+    </row>
+    <row r="234" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A234" s="43">
+        <v>10</v>
+      </c>
+      <c r="B234" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C234" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D234" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E234" s="42">
+        <v>552413.02</v>
+      </c>
+      <c r="F234" s="42">
+        <v>3584644</v>
+      </c>
+      <c r="G234" s="42">
+        <v>2953828.6</v>
+      </c>
+      <c r="H234" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="I234" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="J234" s="42">
+        <v>5</v>
+      </c>
+      <c r="K234" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="L234" s="42">
+        <v>0.1</v>
+      </c>
+      <c r="M234" s="42">
+        <v>0</v>
+      </c>
+      <c r="N234" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O234" s="42">
+        <v>0</v>
+      </c>
+      <c r="P234" s="42">
+        <v>358464.402</v>
+      </c>
+      <c r="Q234" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A235" s="43">
+        <v>11</v>
+      </c>
+      <c r="B235" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C235" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D235" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E235" s="42">
+        <v>552413.02</v>
+      </c>
+      <c r="F235" s="42">
+        <v>3226179.6</v>
+      </c>
+      <c r="G235" s="42">
+        <v>2953828.6</v>
+      </c>
+      <c r="H235" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="I235" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="J235" s="42">
+        <v>6</v>
+      </c>
+      <c r="K235" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="L235" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="M235" s="42">
+        <v>0.02</v>
+      </c>
+      <c r="N235" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O235" s="42">
+        <v>0</v>
+      </c>
+      <c r="P235" s="42">
+        <v>64523.591999999997</v>
+      </c>
+      <c r="Q235" s="42">
+        <v>59076.57</v>
+      </c>
+    </row>
+    <row r="236" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A236" s="43">
+        <v>12</v>
+      </c>
+      <c r="B236" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C236" s="42">
+        <v>303429</v>
+      </c>
+      <c r="D236" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E236" s="42">
+        <v>552413.02</v>
+      </c>
+      <c r="F236" s="42">
+        <v>3161656</v>
+      </c>
+      <c r="G236" s="42">
+        <v>2894752</v>
+      </c>
+      <c r="H236" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="I236" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="J236" s="42">
+        <v>7</v>
+      </c>
+      <c r="K236" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="L236" s="42">
+        <v>0.01</v>
+      </c>
+      <c r="M236" s="42">
+        <v>0</v>
+      </c>
+      <c r="N236" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="O236" s="42">
+        <v>5524.13</v>
+      </c>
+      <c r="P236" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q236" s="42">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>